<commit_message>
Commit code ngày 03/03/2020
</commit_message>
<xml_diff>
--- a/Document/Schedule.xlsx
+++ b/Document/Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QuyenNQ\Documents\Trainning202003\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849EEC92-640A-4D6B-A031-78F9B452EE30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2805FF-5D56-4968-9293-4CF83F2A02FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="26715" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3465" yWindow="1380" windowWidth="21600" windowHeight="14085" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Task name</t>
     <phoneticPr fontId="1"/>
@@ -63,13 +63,10 @@
     <t>Test</t>
   </si>
   <si>
-    <t>Khởi tạo, Chọn trong Combobox, Thực hiện tìm kiếm</t>
+    <t>Thêm, Sửa, Xóa, Lưu</t>
   </si>
   <si>
-    <t>17h30 02/03/2020</t>
-  </si>
-  <si>
-    <t>10h 02/03/2020</t>
+    <t>Tạo Database, Khởi tạo, Chọn trong Combobox, Thực hiện tìm kiếm</t>
   </si>
 </sst>
 </file>
@@ -1092,6 +1089,36 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1129,36 +1156,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1534,7 +1531,7 @@
       <pane xSplit="3" ySplit="8" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1554,8 +1551,8 @@
       <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:38" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="66"/>
-      <c r="B2" s="66"/>
+      <c r="A2" s="76"/>
+      <c r="B2" s="76"/>
       <c r="C2" s="7"/>
       <c r="Y2" s="7"/>
       <c r="Z2" s="7"/>
@@ -1573,8 +1570,8 @@
       <c r="AL2" s="7"/>
     </row>
     <row r="3" spans="1:38" s="5" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A3" s="67"/>
-      <c r="B3" s="67"/>
+      <c r="A3" s="77"/>
+      <c r="B3" s="77"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -1614,66 +1611,66 @@
     </row>
     <row r="4" spans="1:38" s="4" customFormat="1" ht="15.75" thickBot="1"/>
     <row r="5" spans="1:38" ht="15" customHeight="1">
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="69"/>
-      <c r="D5" s="77" t="s">
+      <c r="C5" s="79"/>
+      <c r="D5" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="77" t="s">
+      <c r="E5" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="77" t="s">
+      <c r="F5" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="77" t="s">
+      <c r="G5" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="80" t="s">
+      <c r="H5" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="74" t="s">
+      <c r="I5" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="75"/>
-      <c r="K5" s="75"/>
-      <c r="L5" s="75"/>
-      <c r="M5" s="75"/>
-      <c r="N5" s="75"/>
-      <c r="O5" s="75"/>
-      <c r="P5" s="75"/>
-      <c r="Q5" s="75"/>
-      <c r="R5" s="75"/>
-      <c r="S5" s="75"/>
-      <c r="T5" s="75"/>
-      <c r="U5" s="75"/>
-      <c r="V5" s="75"/>
-      <c r="W5" s="75"/>
-      <c r="X5" s="75"/>
-      <c r="Y5" s="75"/>
-      <c r="Z5" s="75"/>
-      <c r="AA5" s="75"/>
-      <c r="AB5" s="75"/>
-      <c r="AC5" s="75"/>
-      <c r="AD5" s="75"/>
-      <c r="AE5" s="75"/>
-      <c r="AF5" s="75"/>
-      <c r="AG5" s="75"/>
-      <c r="AH5" s="75"/>
-      <c r="AI5" s="75"/>
-      <c r="AJ5" s="75"/>
-      <c r="AK5" s="75"/>
-      <c r="AL5" s="76"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
+      <c r="O5" s="63"/>
+      <c r="P5" s="63"/>
+      <c r="Q5" s="63"/>
+      <c r="R5" s="63"/>
+      <c r="S5" s="63"/>
+      <c r="T5" s="63"/>
+      <c r="U5" s="63"/>
+      <c r="V5" s="63"/>
+      <c r="W5" s="63"/>
+      <c r="X5" s="63"/>
+      <c r="Y5" s="63"/>
+      <c r="Z5" s="63"/>
+      <c r="AA5" s="63"/>
+      <c r="AB5" s="63"/>
+      <c r="AC5" s="63"/>
+      <c r="AD5" s="63"/>
+      <c r="AE5" s="63"/>
+      <c r="AF5" s="63"/>
+      <c r="AG5" s="63"/>
+      <c r="AH5" s="63"/>
+      <c r="AI5" s="63"/>
+      <c r="AJ5" s="63"/>
+      <c r="AK5" s="63"/>
+      <c r="AL5" s="64"/>
     </row>
     <row r="6" spans="1:38">
-      <c r="B6" s="70"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="81"/>
+      <c r="B6" s="80"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="69"/>
       <c r="I6" s="60">
         <v>43892</v>
       </c>
@@ -1766,13 +1763,13 @@
       </c>
     </row>
     <row r="7" spans="1:38" ht="15.75" thickBot="1">
-      <c r="B7" s="72"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
-      <c r="G7" s="79"/>
-      <c r="H7" s="82"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="70"/>
       <c r="I7" s="1" t="str">
         <f>CHOOSE(WEEKDAY(I6),"日","月","火","水","木","金","土")</f>
         <v>月</v>
@@ -1936,22 +1933,26 @@
     </row>
     <row r="9" spans="1:38" ht="26.25" customHeight="1">
       <c r="A9" s="2"/>
-      <c r="B9" s="61" t="s">
+      <c r="B9" s="71" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="H9" s="83">
-        <v>0.2</v>
+      <c r="D9" s="22">
+        <v>43892</v>
+      </c>
+      <c r="E9" s="22">
+        <v>43893</v>
+      </c>
+      <c r="F9" s="22">
+        <v>43892</v>
+      </c>
+      <c r="G9" s="22">
+        <v>43893</v>
+      </c>
+      <c r="H9" s="61">
+        <v>0.9</v>
       </c>
       <c r="I9" s="40"/>
       <c r="J9" s="41"/>
@@ -1986,10 +1987,16 @@
     </row>
     <row r="10" spans="1:38" ht="26.25" customHeight="1">
       <c r="A10" s="2"/>
-      <c r="B10" s="61"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="9">
+        <v>43894</v>
+      </c>
+      <c r="E10" s="9">
+        <v>43896</v>
+      </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="H10" s="10"/>
@@ -2026,7 +2033,7 @@
     </row>
     <row r="11" spans="1:38" ht="26.25" customHeight="1">
       <c r="A11" s="2"/>
-      <c r="B11" s="61"/>
+      <c r="B11" s="71"/>
       <c r="C11" s="33"/>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
@@ -2066,7 +2073,7 @@
     </row>
     <row r="12" spans="1:38" ht="26.25" customHeight="1">
       <c r="A12" s="2"/>
-      <c r="B12" s="62" t="s">
+      <c r="B12" s="72" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="34"/>
@@ -2108,7 +2115,7 @@
     </row>
     <row r="13" spans="1:38" ht="26.25" customHeight="1">
       <c r="A13" s="2"/>
-      <c r="B13" s="62"/>
+      <c r="B13" s="72"/>
       <c r="C13" s="35"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
@@ -2148,7 +2155,7 @@
     </row>
     <row r="14" spans="1:38" ht="26.25" customHeight="1">
       <c r="A14" s="2"/>
-      <c r="B14" s="62"/>
+      <c r="B14" s="72"/>
       <c r="C14" s="36"/>
       <c r="D14" s="29"/>
       <c r="E14" s="29"/>
@@ -2188,7 +2195,7 @@
     </row>
     <row r="15" spans="1:38" ht="26.25" customHeight="1">
       <c r="A15" s="15"/>
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="73" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="37"/>
@@ -2230,7 +2237,7 @@
     </row>
     <row r="16" spans="1:38" ht="26.25" customHeight="1">
       <c r="A16" s="15"/>
-      <c r="B16" s="64"/>
+      <c r="B16" s="74"/>
       <c r="C16" s="38"/>
       <c r="D16" s="13"/>
       <c r="E16" s="14"/>
@@ -2270,7 +2277,7 @@
     </row>
     <row r="17" spans="1:38" ht="26.25" customHeight="1" thickBot="1">
       <c r="A17" s="15"/>
-      <c r="B17" s="65"/>
+      <c r="B17" s="75"/>
       <c r="C17" s="39"/>
       <c r="D17" s="19"/>
       <c r="E17" s="20"/>
@@ -2310,17 +2317,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="B5:C7"/>
     <mergeCell ref="I5:AL5"/>
     <mergeCell ref="D5:D7"/>
     <mergeCell ref="E5:E7"/>
     <mergeCell ref="F5:F7"/>
     <mergeCell ref="G5:G7"/>
     <mergeCell ref="H5:H7"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="B5:C7"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="H15:H17 H9:H10">

</xml_diff>

<commit_message>
Commit code ngày 04/03/2020
</commit_message>
<xml_diff>
--- a/Document/Schedule.xlsx
+++ b/Document/Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QuyenNQ\Documents\Trainning202003\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2805FF-5D56-4968-9293-4CF83F2A02FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E4E567-9664-436B-8C27-8C60B7F56041}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="1380" windowWidth="21600" windowHeight="14085" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="1035" windowWidth="21600" windowHeight="14085" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Task name</t>
     <phoneticPr fontId="1"/>
@@ -63,10 +63,28 @@
     <t>Test</t>
   </si>
   <si>
-    <t>Thêm, Sửa, Xóa, Lưu</t>
+    <t>Thực hiện tìm kiếm</t>
   </si>
   <si>
-    <t>Tạo Database, Khởi tạo, Chọn trong Combobox, Thực hiện tìm kiếm</t>
+    <t>Chọn trong Combobox</t>
+  </si>
+  <si>
+    <t>Khởi tạo</t>
+  </si>
+  <si>
+    <t>Tạo Database</t>
+  </si>
+  <si>
+    <t>Thêm</t>
+  </si>
+  <si>
+    <t>Xóa</t>
+  </si>
+  <si>
+    <t>Lưu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sửa</t>
   </si>
 </sst>
 </file>
@@ -173,7 +191,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="58">
+  <borders count="66">
     <border>
       <left/>
       <right/>
@@ -898,6 +916,96 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -905,7 +1013,7 @@
     </xf>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1092,6 +1200,42 @@
     <xf numFmtId="9" fontId="4" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1119,44 +1263,41 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="62" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1525,13 +1666,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL17"/>
+  <dimension ref="A1:AL23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="8" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1551,8 +1692,8 @@
       <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:38" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="76"/>
-      <c r="B2" s="76"/>
+      <c r="A2" s="66"/>
+      <c r="B2" s="66"/>
       <c r="C2" s="7"/>
       <c r="Y2" s="7"/>
       <c r="Z2" s="7"/>
@@ -1570,8 +1711,8 @@
       <c r="AL2" s="7"/>
     </row>
     <row r="3" spans="1:38" s="5" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A3" s="77"/>
-      <c r="B3" s="77"/>
+      <c r="A3" s="67"/>
+      <c r="B3" s="67"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -1611,66 +1752,66 @@
     </row>
     <row r="4" spans="1:38" s="4" customFormat="1" ht="15.75" thickBot="1"/>
     <row r="5" spans="1:38" ht="15" customHeight="1">
-      <c r="B5" s="78" t="s">
+      <c r="B5" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="79"/>
-      <c r="D5" s="65" t="s">
+      <c r="C5" s="69"/>
+      <c r="D5" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="65" t="s">
+      <c r="E5" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="65" t="s">
+      <c r="F5" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="65" t="s">
+      <c r="G5" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="68" t="s">
+      <c r="H5" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="62" t="s">
+      <c r="I5" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="63"/>
-      <c r="K5" s="63"/>
-      <c r="L5" s="63"/>
-      <c r="M5" s="63"/>
-      <c r="N5" s="63"/>
-      <c r="O5" s="63"/>
-      <c r="P5" s="63"/>
-      <c r="Q5" s="63"/>
-      <c r="R5" s="63"/>
-      <c r="S5" s="63"/>
-      <c r="T5" s="63"/>
-      <c r="U5" s="63"/>
-      <c r="V5" s="63"/>
-      <c r="W5" s="63"/>
-      <c r="X5" s="63"/>
-      <c r="Y5" s="63"/>
-      <c r="Z5" s="63"/>
-      <c r="AA5" s="63"/>
-      <c r="AB5" s="63"/>
-      <c r="AC5" s="63"/>
-      <c r="AD5" s="63"/>
-      <c r="AE5" s="63"/>
-      <c r="AF5" s="63"/>
-      <c r="AG5" s="63"/>
-      <c r="AH5" s="63"/>
-      <c r="AI5" s="63"/>
-      <c r="AJ5" s="63"/>
-      <c r="AK5" s="63"/>
-      <c r="AL5" s="64"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="75"/>
+      <c r="L5" s="75"/>
+      <c r="M5" s="75"/>
+      <c r="N5" s="75"/>
+      <c r="O5" s="75"/>
+      <c r="P5" s="75"/>
+      <c r="Q5" s="75"/>
+      <c r="R5" s="75"/>
+      <c r="S5" s="75"/>
+      <c r="T5" s="75"/>
+      <c r="U5" s="75"/>
+      <c r="V5" s="75"/>
+      <c r="W5" s="75"/>
+      <c r="X5" s="75"/>
+      <c r="Y5" s="75"/>
+      <c r="Z5" s="75"/>
+      <c r="AA5" s="75"/>
+      <c r="AB5" s="75"/>
+      <c r="AC5" s="75"/>
+      <c r="AD5" s="75"/>
+      <c r="AE5" s="75"/>
+      <c r="AF5" s="75"/>
+      <c r="AG5" s="75"/>
+      <c r="AH5" s="75"/>
+      <c r="AI5" s="75"/>
+      <c r="AJ5" s="75"/>
+      <c r="AK5" s="75"/>
+      <c r="AL5" s="76"/>
     </row>
     <row r="6" spans="1:38">
-      <c r="B6" s="80"/>
-      <c r="C6" s="81"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="69"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="81"/>
       <c r="I6" s="60">
         <v>43892</v>
       </c>
@@ -1763,13 +1904,13 @@
       </c>
     </row>
     <row r="7" spans="1:38" ht="15.75" thickBot="1">
-      <c r="B7" s="82"/>
-      <c r="C7" s="83"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="70"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="79"/>
+      <c r="G7" s="79"/>
+      <c r="H7" s="82"/>
       <c r="I7" s="1" t="str">
         <f>CHOOSE(WEEKDAY(I6),"日","月","火","水","木","金","土")</f>
         <v>月</v>
@@ -1933,11 +2074,11 @@
     </row>
     <row r="9" spans="1:38" ht="26.25" customHeight="1">
       <c r="A9" s="2"/>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="62" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D9" s="22">
         <v>43892</v>
@@ -1952,7 +2093,7 @@
         <v>43893</v>
       </c>
       <c r="H9" s="61">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="I9" s="40"/>
       <c r="J9" s="41"/>
@@ -1987,350 +2128,650 @@
     </row>
     <row r="10" spans="1:38" ht="26.25" customHeight="1">
       <c r="A10" s="2"/>
-      <c r="B10" s="71"/>
-      <c r="C10" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="9">
-        <v>43894</v>
-      </c>
-      <c r="E10" s="9">
-        <v>43896</v>
-      </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="44"/>
-      <c r="M10" s="44"/>
-      <c r="N10" s="44"/>
-      <c r="O10" s="44"/>
-      <c r="P10" s="44"/>
-      <c r="Q10" s="44"/>
-      <c r="R10" s="44"/>
-      <c r="S10" s="44"/>
-      <c r="T10" s="44"/>
-      <c r="U10" s="44"/>
-      <c r="V10" s="44"/>
-      <c r="W10" s="44"/>
-      <c r="X10" s="44"/>
-      <c r="Y10" s="44"/>
-      <c r="Z10" s="44"/>
-      <c r="AA10" s="44"/>
-      <c r="AB10" s="44"/>
-      <c r="AC10" s="44"/>
-      <c r="AD10" s="44"/>
-      <c r="AE10" s="44"/>
-      <c r="AF10" s="44"/>
-      <c r="AG10" s="44"/>
-      <c r="AH10" s="44"/>
-      <c r="AI10" s="44"/>
-      <c r="AJ10" s="44"/>
-      <c r="AK10" s="44"/>
-      <c r="AL10" s="45"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="86" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="87">
+        <v>43892</v>
+      </c>
+      <c r="E10" s="87">
+        <v>43893</v>
+      </c>
+      <c r="F10" s="87">
+        <v>43892</v>
+      </c>
+      <c r="G10" s="87">
+        <v>43893</v>
+      </c>
+      <c r="H10" s="88">
+        <v>1</v>
+      </c>
+      <c r="I10" s="49"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="50"/>
+      <c r="N10" s="50"/>
+      <c r="O10" s="50"/>
+      <c r="P10" s="50"/>
+      <c r="Q10" s="50"/>
+      <c r="R10" s="50"/>
+      <c r="S10" s="50"/>
+      <c r="T10" s="50"/>
+      <c r="U10" s="50"/>
+      <c r="V10" s="50"/>
+      <c r="W10" s="50"/>
+      <c r="X10" s="50"/>
+      <c r="Y10" s="50"/>
+      <c r="Z10" s="50"/>
+      <c r="AA10" s="50"/>
+      <c r="AB10" s="50"/>
+      <c r="AC10" s="50"/>
+      <c r="AD10" s="50"/>
+      <c r="AE10" s="50"/>
+      <c r="AF10" s="50"/>
+      <c r="AG10" s="50"/>
+      <c r="AH10" s="50"/>
+      <c r="AI10" s="50"/>
+      <c r="AJ10" s="50"/>
+      <c r="AK10" s="50"/>
+      <c r="AL10" s="51"/>
     </row>
     <row r="11" spans="1:38" ht="26.25" customHeight="1">
       <c r="A11" s="2"/>
-      <c r="B11" s="71"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="46"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="47"/>
-      <c r="L11" s="47"/>
-      <c r="M11" s="47"/>
-      <c r="N11" s="47"/>
-      <c r="O11" s="47"/>
-      <c r="P11" s="47"/>
-      <c r="Q11" s="47"/>
-      <c r="R11" s="47"/>
-      <c r="S11" s="47"/>
-      <c r="T11" s="47"/>
-      <c r="U11" s="47"/>
-      <c r="V11" s="47"/>
-      <c r="W11" s="47"/>
-      <c r="X11" s="47"/>
-      <c r="Y11" s="47"/>
-      <c r="Z11" s="47"/>
-      <c r="AA11" s="47"/>
-      <c r="AB11" s="47"/>
-      <c r="AC11" s="47"/>
-      <c r="AD11" s="47"/>
-      <c r="AE11" s="47"/>
-      <c r="AF11" s="47"/>
-      <c r="AG11" s="47"/>
-      <c r="AH11" s="47"/>
-      <c r="AI11" s="47"/>
-      <c r="AJ11" s="47"/>
-      <c r="AK11" s="47"/>
-      <c r="AL11" s="48"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="86" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="87">
+        <v>43892</v>
+      </c>
+      <c r="E11" s="87">
+        <v>43893</v>
+      </c>
+      <c r="F11" s="87">
+        <v>43892</v>
+      </c>
+      <c r="G11" s="87">
+        <v>43893</v>
+      </c>
+      <c r="H11" s="88">
+        <v>1</v>
+      </c>
+      <c r="I11" s="49"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="50"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="50"/>
+      <c r="P11" s="50"/>
+      <c r="Q11" s="50"/>
+      <c r="R11" s="50"/>
+      <c r="S11" s="50"/>
+      <c r="T11" s="50"/>
+      <c r="U11" s="50"/>
+      <c r="V11" s="50"/>
+      <c r="W11" s="50"/>
+      <c r="X11" s="50"/>
+      <c r="Y11" s="50"/>
+      <c r="Z11" s="50"/>
+      <c r="AA11" s="50"/>
+      <c r="AB11" s="50"/>
+      <c r="AC11" s="50"/>
+      <c r="AD11" s="50"/>
+      <c r="AE11" s="50"/>
+      <c r="AF11" s="50"/>
+      <c r="AG11" s="50"/>
+      <c r="AH11" s="50"/>
+      <c r="AI11" s="50"/>
+      <c r="AJ11" s="50"/>
+      <c r="AK11" s="50"/>
+      <c r="AL11" s="51"/>
     </row>
     <row r="12" spans="1:38" ht="26.25" customHeight="1">
       <c r="A12" s="2"/>
-      <c r="B12" s="72" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="34"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="41"/>
-      <c r="O12" s="41"/>
-      <c r="P12" s="41"/>
-      <c r="Q12" s="41"/>
-      <c r="R12" s="41"/>
-      <c r="S12" s="41"/>
-      <c r="T12" s="41"/>
-      <c r="U12" s="41"/>
-      <c r="V12" s="41"/>
-      <c r="W12" s="41"/>
-      <c r="X12" s="41"/>
-      <c r="Y12" s="41"/>
-      <c r="Z12" s="41"/>
-      <c r="AA12" s="41"/>
-      <c r="AB12" s="41"/>
-      <c r="AC12" s="41"/>
-      <c r="AD12" s="41"/>
-      <c r="AE12" s="41"/>
-      <c r="AF12" s="41"/>
-      <c r="AG12" s="41"/>
-      <c r="AH12" s="41"/>
-      <c r="AI12" s="41"/>
-      <c r="AJ12" s="41"/>
-      <c r="AK12" s="41"/>
-      <c r="AL12" s="42"/>
+      <c r="B12" s="62"/>
+      <c r="C12" s="86" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="87">
+        <v>43892</v>
+      </c>
+      <c r="E12" s="87">
+        <v>43893</v>
+      </c>
+      <c r="F12" s="87">
+        <v>43892</v>
+      </c>
+      <c r="G12" s="87">
+        <v>43893</v>
+      </c>
+      <c r="H12" s="88">
+        <v>1</v>
+      </c>
+      <c r="I12" s="49"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="50"/>
+      <c r="P12" s="50"/>
+      <c r="Q12" s="50"/>
+      <c r="R12" s="50"/>
+      <c r="S12" s="50"/>
+      <c r="T12" s="50"/>
+      <c r="U12" s="50"/>
+      <c r="V12" s="50"/>
+      <c r="W12" s="50"/>
+      <c r="X12" s="50"/>
+      <c r="Y12" s="50"/>
+      <c r="Z12" s="50"/>
+      <c r="AA12" s="50"/>
+      <c r="AB12" s="50"/>
+      <c r="AC12" s="50"/>
+      <c r="AD12" s="50"/>
+      <c r="AE12" s="50"/>
+      <c r="AF12" s="50"/>
+      <c r="AG12" s="50"/>
+      <c r="AH12" s="50"/>
+      <c r="AI12" s="50"/>
+      <c r="AJ12" s="50"/>
+      <c r="AK12" s="50"/>
+      <c r="AL12" s="51"/>
     </row>
     <row r="13" spans="1:38" ht="26.25" customHeight="1">
       <c r="A13" s="2"/>
-      <c r="B13" s="72"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="44"/>
-      <c r="L13" s="44"/>
-      <c r="M13" s="44"/>
-      <c r="N13" s="44"/>
-      <c r="O13" s="44"/>
-      <c r="P13" s="44"/>
-      <c r="Q13" s="44"/>
-      <c r="R13" s="44"/>
-      <c r="S13" s="44"/>
-      <c r="T13" s="44"/>
-      <c r="U13" s="44"/>
-      <c r="V13" s="44"/>
-      <c r="W13" s="44"/>
-      <c r="X13" s="44"/>
-      <c r="Y13" s="44"/>
-      <c r="Z13" s="44"/>
-      <c r="AA13" s="44"/>
-      <c r="AB13" s="44"/>
-      <c r="AC13" s="44"/>
-      <c r="AD13" s="44"/>
-      <c r="AE13" s="44"/>
-      <c r="AF13" s="44"/>
-      <c r="AG13" s="44"/>
-      <c r="AH13" s="44"/>
-      <c r="AI13" s="44"/>
-      <c r="AJ13" s="44"/>
-      <c r="AK13" s="44"/>
-      <c r="AL13" s="45"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="86" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="87">
+        <v>43894</v>
+      </c>
+      <c r="E13" s="87">
+        <v>43895</v>
+      </c>
+      <c r="F13" s="87">
+        <v>43894</v>
+      </c>
+      <c r="G13" s="87"/>
+      <c r="H13" s="88"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="50"/>
+      <c r="O13" s="50"/>
+      <c r="P13" s="50"/>
+      <c r="Q13" s="50"/>
+      <c r="R13" s="50"/>
+      <c r="S13" s="50"/>
+      <c r="T13" s="50"/>
+      <c r="U13" s="50"/>
+      <c r="V13" s="50"/>
+      <c r="W13" s="50"/>
+      <c r="X13" s="50"/>
+      <c r="Y13" s="50"/>
+      <c r="Z13" s="50"/>
+      <c r="AA13" s="50"/>
+      <c r="AB13" s="50"/>
+      <c r="AC13" s="50"/>
+      <c r="AD13" s="50"/>
+      <c r="AE13" s="50"/>
+      <c r="AF13" s="50"/>
+      <c r="AG13" s="50"/>
+      <c r="AH13" s="50"/>
+      <c r="AI13" s="50"/>
+      <c r="AJ13" s="50"/>
+      <c r="AK13" s="50"/>
+      <c r="AL13" s="51"/>
     </row>
     <row r="14" spans="1:38" ht="26.25" customHeight="1">
       <c r="A14" s="2"/>
-      <c r="B14" s="72"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="47"/>
-      <c r="K14" s="47"/>
-      <c r="L14" s="47"/>
-      <c r="M14" s="47"/>
-      <c r="N14" s="47"/>
-      <c r="O14" s="47"/>
-      <c r="P14" s="47"/>
-      <c r="Q14" s="47"/>
-      <c r="R14" s="47"/>
-      <c r="S14" s="47"/>
-      <c r="T14" s="47"/>
-      <c r="U14" s="47"/>
-      <c r="V14" s="47"/>
-      <c r="W14" s="47"/>
-      <c r="X14" s="47"/>
-      <c r="Y14" s="47"/>
-      <c r="Z14" s="47"/>
-      <c r="AA14" s="47"/>
-      <c r="AB14" s="47"/>
-      <c r="AC14" s="47"/>
-      <c r="AD14" s="47"/>
-      <c r="AE14" s="47"/>
-      <c r="AF14" s="47"/>
-      <c r="AG14" s="47"/>
-      <c r="AH14" s="47"/>
-      <c r="AI14" s="47"/>
-      <c r="AJ14" s="47"/>
-      <c r="AK14" s="47"/>
-      <c r="AL14" s="48"/>
+      <c r="B14" s="62"/>
+      <c r="C14" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="9">
+        <v>43894</v>
+      </c>
+      <c r="E14" s="9">
+        <v>43895</v>
+      </c>
+      <c r="F14" s="9">
+        <v>43894</v>
+      </c>
+      <c r="G14" s="9"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="44"/>
+      <c r="L14" s="44"/>
+      <c r="M14" s="44"/>
+      <c r="N14" s="44"/>
+      <c r="O14" s="44"/>
+      <c r="P14" s="44"/>
+      <c r="Q14" s="44"/>
+      <c r="R14" s="44"/>
+      <c r="S14" s="44"/>
+      <c r="T14" s="44"/>
+      <c r="U14" s="44"/>
+      <c r="V14" s="44"/>
+      <c r="W14" s="44"/>
+      <c r="X14" s="44"/>
+      <c r="Y14" s="44"/>
+      <c r="Z14" s="44"/>
+      <c r="AA14" s="44"/>
+      <c r="AB14" s="44"/>
+      <c r="AC14" s="44"/>
+      <c r="AD14" s="44"/>
+      <c r="AE14" s="44"/>
+      <c r="AF14" s="44"/>
+      <c r="AG14" s="44"/>
+      <c r="AH14" s="44"/>
+      <c r="AI14" s="44"/>
+      <c r="AJ14" s="44"/>
+      <c r="AK14" s="44"/>
+      <c r="AL14" s="45"/>
     </row>
     <row r="15" spans="1:38" ht="26.25" customHeight="1">
-      <c r="A15" s="15"/>
-      <c r="B15" s="73" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="50"/>
-      <c r="K15" s="50"/>
-      <c r="L15" s="50"/>
-      <c r="M15" s="50"/>
-      <c r="N15" s="50"/>
-      <c r="O15" s="50"/>
-      <c r="P15" s="50"/>
-      <c r="Q15" s="50"/>
-      <c r="R15" s="50"/>
-      <c r="S15" s="50"/>
-      <c r="T15" s="50"/>
-      <c r="U15" s="50"/>
-      <c r="V15" s="50"/>
-      <c r="W15" s="50"/>
-      <c r="X15" s="50"/>
-      <c r="Y15" s="50"/>
-      <c r="Z15" s="50"/>
-      <c r="AA15" s="50"/>
-      <c r="AB15" s="50"/>
-      <c r="AC15" s="50"/>
-      <c r="AD15" s="50"/>
-      <c r="AE15" s="50"/>
-      <c r="AF15" s="50"/>
-      <c r="AG15" s="50"/>
-      <c r="AH15" s="50"/>
-      <c r="AI15" s="50"/>
-      <c r="AJ15" s="50"/>
-      <c r="AK15" s="50"/>
-      <c r="AL15" s="51"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="89" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="90">
+        <v>43895</v>
+      </c>
+      <c r="E15" s="90">
+        <v>43896</v>
+      </c>
+      <c r="F15" s="90">
+        <v>43894</v>
+      </c>
+      <c r="G15" s="90"/>
+      <c r="H15" s="91"/>
+      <c r="I15" s="92"/>
+      <c r="J15" s="93"/>
+      <c r="K15" s="93"/>
+      <c r="L15" s="93"/>
+      <c r="M15" s="93"/>
+      <c r="N15" s="93"/>
+      <c r="O15" s="93"/>
+      <c r="P15" s="93"/>
+      <c r="Q15" s="93"/>
+      <c r="R15" s="93"/>
+      <c r="S15" s="93"/>
+      <c r="T15" s="93"/>
+      <c r="U15" s="93"/>
+      <c r="V15" s="93"/>
+      <c r="W15" s="93"/>
+      <c r="X15" s="93"/>
+      <c r="Y15" s="93"/>
+      <c r="Z15" s="93"/>
+      <c r="AA15" s="93"/>
+      <c r="AB15" s="93"/>
+      <c r="AC15" s="93"/>
+      <c r="AD15" s="93"/>
+      <c r="AE15" s="93"/>
+      <c r="AF15" s="93"/>
+      <c r="AG15" s="93"/>
+      <c r="AH15" s="93"/>
+      <c r="AI15" s="93"/>
+      <c r="AJ15" s="93"/>
+      <c r="AK15" s="93"/>
+      <c r="AL15" s="94"/>
     </row>
     <row r="16" spans="1:38" ht="26.25" customHeight="1">
-      <c r="A16" s="15"/>
-      <c r="B16" s="74"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="44"/>
-      <c r="K16" s="52"/>
-      <c r="L16" s="52"/>
-      <c r="M16" s="52"/>
-      <c r="N16" s="52"/>
-      <c r="O16" s="44"/>
-      <c r="P16" s="44"/>
-      <c r="Q16" s="52"/>
-      <c r="R16" s="52"/>
-      <c r="S16" s="52"/>
-      <c r="T16" s="52"/>
-      <c r="U16" s="52"/>
-      <c r="V16" s="44"/>
-      <c r="W16" s="44"/>
-      <c r="X16" s="52"/>
-      <c r="Y16" s="52"/>
-      <c r="Z16" s="52"/>
-      <c r="AA16" s="52"/>
-      <c r="AB16" s="52"/>
-      <c r="AC16" s="44"/>
-      <c r="AD16" s="44"/>
-      <c r="AE16" s="52"/>
-      <c r="AF16" s="52"/>
-      <c r="AG16" s="52"/>
-      <c r="AH16" s="52"/>
-      <c r="AI16" s="52"/>
-      <c r="AJ16" s="44"/>
-      <c r="AK16" s="44"/>
-      <c r="AL16" s="53"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="62"/>
+      <c r="C16" s="89" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="90">
+        <v>43895</v>
+      </c>
+      <c r="E16" s="90">
+        <v>43896</v>
+      </c>
+      <c r="F16" s="90"/>
+      <c r="G16" s="90"/>
+      <c r="H16" s="91"/>
+      <c r="I16" s="92"/>
+      <c r="J16" s="93"/>
+      <c r="K16" s="93"/>
+      <c r="L16" s="93"/>
+      <c r="M16" s="93"/>
+      <c r="N16" s="93"/>
+      <c r="O16" s="93"/>
+      <c r="P16" s="93"/>
+      <c r="Q16" s="93"/>
+      <c r="R16" s="93"/>
+      <c r="S16" s="93"/>
+      <c r="T16" s="93"/>
+      <c r="U16" s="93"/>
+      <c r="V16" s="93"/>
+      <c r="W16" s="93"/>
+      <c r="X16" s="93"/>
+      <c r="Y16" s="93"/>
+      <c r="Z16" s="93"/>
+      <c r="AA16" s="93"/>
+      <c r="AB16" s="93"/>
+      <c r="AC16" s="93"/>
+      <c r="AD16" s="93"/>
+      <c r="AE16" s="93"/>
+      <c r="AF16" s="93"/>
+      <c r="AG16" s="93"/>
+      <c r="AH16" s="93"/>
+      <c r="AI16" s="93"/>
+      <c r="AJ16" s="93"/>
+      <c r="AK16" s="93"/>
+      <c r="AL16" s="94"/>
     </row>
-    <row r="17" spans="1:38" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A17" s="15"/>
-      <c r="B17" s="75"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54"/>
-      <c r="K17" s="55"/>
-      <c r="L17" s="55"/>
-      <c r="M17" s="55"/>
-      <c r="N17" s="55"/>
-      <c r="O17" s="54"/>
-      <c r="P17" s="54"/>
-      <c r="Q17" s="55"/>
-      <c r="R17" s="55"/>
-      <c r="S17" s="55"/>
-      <c r="T17" s="55"/>
-      <c r="U17" s="55"/>
-      <c r="V17" s="54"/>
-      <c r="W17" s="54"/>
-      <c r="X17" s="55"/>
-      <c r="Y17" s="55"/>
-      <c r="Z17" s="55"/>
-      <c r="AA17" s="55"/>
-      <c r="AB17" s="55"/>
-      <c r="AC17" s="54"/>
-      <c r="AD17" s="54"/>
-      <c r="AE17" s="55"/>
-      <c r="AF17" s="55"/>
-      <c r="AG17" s="55"/>
-      <c r="AH17" s="55"/>
-      <c r="AI17" s="55"/>
-      <c r="AJ17" s="54"/>
-      <c r="AK17" s="54"/>
-      <c r="AL17" s="56"/>
+    <row r="17" spans="1:38" ht="26.25" customHeight="1">
+      <c r="A17" s="2"/>
+      <c r="B17" s="62"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="47"/>
+      <c r="K17" s="47"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="47"/>
+      <c r="O17" s="47"/>
+      <c r="P17" s="47"/>
+      <c r="Q17" s="47"/>
+      <c r="R17" s="47"/>
+      <c r="S17" s="47"/>
+      <c r="T17" s="47"/>
+      <c r="U17" s="47"/>
+      <c r="V17" s="47"/>
+      <c r="W17" s="47"/>
+      <c r="X17" s="47"/>
+      <c r="Y17" s="47"/>
+      <c r="Z17" s="47"/>
+      <c r="AA17" s="47"/>
+      <c r="AB17" s="47"/>
+      <c r="AC17" s="47"/>
+      <c r="AD17" s="47"/>
+      <c r="AE17" s="47"/>
+      <c r="AF17" s="47"/>
+      <c r="AG17" s="47"/>
+      <c r="AH17" s="47"/>
+      <c r="AI17" s="47"/>
+      <c r="AJ17" s="47"/>
+      <c r="AK17" s="47"/>
+      <c r="AL17" s="48"/>
+    </row>
+    <row r="18" spans="1:38" ht="26.25" customHeight="1">
+      <c r="A18" s="2"/>
+      <c r="B18" s="83" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="34"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="41"/>
+      <c r="L18" s="41"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="41"/>
+      <c r="P18" s="41"/>
+      <c r="Q18" s="41"/>
+      <c r="R18" s="41"/>
+      <c r="S18" s="41"/>
+      <c r="T18" s="41"/>
+      <c r="U18" s="41"/>
+      <c r="V18" s="41"/>
+      <c r="W18" s="41"/>
+      <c r="X18" s="41"/>
+      <c r="Y18" s="41"/>
+      <c r="Z18" s="41"/>
+      <c r="AA18" s="41"/>
+      <c r="AB18" s="41"/>
+      <c r="AC18" s="41"/>
+      <c r="AD18" s="41"/>
+      <c r="AE18" s="41"/>
+      <c r="AF18" s="41"/>
+      <c r="AG18" s="41"/>
+      <c r="AH18" s="41"/>
+      <c r="AI18" s="41"/>
+      <c r="AJ18" s="41"/>
+      <c r="AK18" s="41"/>
+      <c r="AL18" s="42"/>
+    </row>
+    <row r="19" spans="1:38" ht="26.25" customHeight="1">
+      <c r="A19" s="2"/>
+      <c r="B19" s="84"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="44"/>
+      <c r="L19" s="44"/>
+      <c r="M19" s="44"/>
+      <c r="N19" s="44"/>
+      <c r="O19" s="44"/>
+      <c r="P19" s="44"/>
+      <c r="Q19" s="44"/>
+      <c r="R19" s="44"/>
+      <c r="S19" s="44"/>
+      <c r="T19" s="44"/>
+      <c r="U19" s="44"/>
+      <c r="V19" s="44"/>
+      <c r="W19" s="44"/>
+      <c r="X19" s="44"/>
+      <c r="Y19" s="44"/>
+      <c r="Z19" s="44"/>
+      <c r="AA19" s="44"/>
+      <c r="AB19" s="44"/>
+      <c r="AC19" s="44"/>
+      <c r="AD19" s="44"/>
+      <c r="AE19" s="44"/>
+      <c r="AF19" s="44"/>
+      <c r="AG19" s="44"/>
+      <c r="AH19" s="44"/>
+      <c r="AI19" s="44"/>
+      <c r="AJ19" s="44"/>
+      <c r="AK19" s="44"/>
+      <c r="AL19" s="45"/>
+    </row>
+    <row r="20" spans="1:38" ht="26.25" customHeight="1">
+      <c r="A20" s="2"/>
+      <c r="B20" s="85"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="47"/>
+      <c r="N20" s="47"/>
+      <c r="O20" s="47"/>
+      <c r="P20" s="47"/>
+      <c r="Q20" s="47"/>
+      <c r="R20" s="47"/>
+      <c r="S20" s="47"/>
+      <c r="T20" s="47"/>
+      <c r="U20" s="47"/>
+      <c r="V20" s="47"/>
+      <c r="W20" s="47"/>
+      <c r="X20" s="47"/>
+      <c r="Y20" s="47"/>
+      <c r="Z20" s="47"/>
+      <c r="AA20" s="47"/>
+      <c r="AB20" s="47"/>
+      <c r="AC20" s="47"/>
+      <c r="AD20" s="47"/>
+      <c r="AE20" s="47"/>
+      <c r="AF20" s="47"/>
+      <c r="AG20" s="47"/>
+      <c r="AH20" s="47"/>
+      <c r="AI20" s="47"/>
+      <c r="AJ20" s="47"/>
+      <c r="AK20" s="47"/>
+      <c r="AL20" s="48"/>
+    </row>
+    <row r="21" spans="1:38" ht="26.25" customHeight="1">
+      <c r="A21" s="15"/>
+      <c r="B21" s="63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="37"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="50"/>
+      <c r="L21" s="50"/>
+      <c r="M21" s="50"/>
+      <c r="N21" s="50"/>
+      <c r="O21" s="50"/>
+      <c r="P21" s="50"/>
+      <c r="Q21" s="50"/>
+      <c r="R21" s="50"/>
+      <c r="S21" s="50"/>
+      <c r="T21" s="50"/>
+      <c r="U21" s="50"/>
+      <c r="V21" s="50"/>
+      <c r="W21" s="50"/>
+      <c r="X21" s="50"/>
+      <c r="Y21" s="50"/>
+      <c r="Z21" s="50"/>
+      <c r="AA21" s="50"/>
+      <c r="AB21" s="50"/>
+      <c r="AC21" s="50"/>
+      <c r="AD21" s="50"/>
+      <c r="AE21" s="50"/>
+      <c r="AF21" s="50"/>
+      <c r="AG21" s="50"/>
+      <c r="AH21" s="50"/>
+      <c r="AI21" s="50"/>
+      <c r="AJ21" s="50"/>
+      <c r="AK21" s="50"/>
+      <c r="AL21" s="51"/>
+    </row>
+    <row r="22" spans="1:38" ht="26.25" customHeight="1">
+      <c r="A22" s="15"/>
+      <c r="B22" s="64"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="52"/>
+      <c r="L22" s="52"/>
+      <c r="M22" s="52"/>
+      <c r="N22" s="52"/>
+      <c r="O22" s="44"/>
+      <c r="P22" s="44"/>
+      <c r="Q22" s="52"/>
+      <c r="R22" s="52"/>
+      <c r="S22" s="52"/>
+      <c r="T22" s="52"/>
+      <c r="U22" s="52"/>
+      <c r="V22" s="44"/>
+      <c r="W22" s="44"/>
+      <c r="X22" s="52"/>
+      <c r="Y22" s="52"/>
+      <c r="Z22" s="52"/>
+      <c r="AA22" s="52"/>
+      <c r="AB22" s="52"/>
+      <c r="AC22" s="44"/>
+      <c r="AD22" s="44"/>
+      <c r="AE22" s="52"/>
+      <c r="AF22" s="52"/>
+      <c r="AG22" s="52"/>
+      <c r="AH22" s="52"/>
+      <c r="AI22" s="52"/>
+      <c r="AJ22" s="44"/>
+      <c r="AK22" s="44"/>
+      <c r="AL22" s="53"/>
+    </row>
+    <row r="23" spans="1:38" ht="26.25" customHeight="1" thickBot="1">
+      <c r="A23" s="15"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="54"/>
+      <c r="K23" s="55"/>
+      <c r="L23" s="55"/>
+      <c r="M23" s="55"/>
+      <c r="N23" s="55"/>
+      <c r="O23" s="54"/>
+      <c r="P23" s="54"/>
+      <c r="Q23" s="55"/>
+      <c r="R23" s="55"/>
+      <c r="S23" s="55"/>
+      <c r="T23" s="55"/>
+      <c r="U23" s="55"/>
+      <c r="V23" s="54"/>
+      <c r="W23" s="54"/>
+      <c r="X23" s="55"/>
+      <c r="Y23" s="55"/>
+      <c r="Z23" s="55"/>
+      <c r="AA23" s="55"/>
+      <c r="AB23" s="55"/>
+      <c r="AC23" s="54"/>
+      <c r="AD23" s="54"/>
+      <c r="AE23" s="55"/>
+      <c r="AF23" s="55"/>
+      <c r="AG23" s="55"/>
+      <c r="AH23" s="55"/>
+      <c r="AI23" s="55"/>
+      <c r="AJ23" s="54"/>
+      <c r="AK23" s="54"/>
+      <c r="AL23" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="B5:C7"/>
     <mergeCell ref="I5:AL5"/>
     <mergeCell ref="D5:D7"/>
     <mergeCell ref="E5:E7"/>
     <mergeCell ref="F5:F7"/>
     <mergeCell ref="G5:G7"/>
     <mergeCell ref="H5:H7"/>
+    <mergeCell ref="B9:B17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="B5:C7"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
-  <conditionalFormatting sqref="H15:H17 H9:H10">
+  <conditionalFormatting sqref="H21:H23 H9:H16">
     <cfRule type="dataBar" priority="10">
       <dataBar>
         <cfvo type="num" val="1"/>
@@ -2344,7 +2785,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I9:AL17">
+  <conditionalFormatting sqref="I9:AL23">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>WEEKDAY(I$6,2)&gt;5</formula>
     </cfRule>
@@ -2365,7 +2806,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H12:H13">
+  <conditionalFormatting sqref="H18:H19">
     <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="num" val="1"/>
@@ -2397,7 +2838,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H15:H17 H9:H10</xm:sqref>
+          <xm:sqref>H21:H23 H9:H16</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{30D8C443-C769-49A2-8D0C-94AB7C153FB3}">
@@ -2412,7 +2853,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H12:H13</xm:sqref>
+          <xm:sqref>H18:H19</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Commit code ngày 2020/03/05
</commit_message>
<xml_diff>
--- a/Document/Schedule.xlsx
+++ b/Document/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QuyenNQ\Documents\Trainning202003\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E4E567-9664-436B-8C27-8C60B7F56041}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6EFDAD-F9E3-498F-B7BD-A22FB86980D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="1035" windowWidth="21600" windowHeight="14085" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1044,9 +1044,6 @@
     <xf numFmtId="165" fontId="2" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="2" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1200,7 +1197,67 @@
     <xf numFmtId="9" fontId="4" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1236,68 +1293,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="4" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="62" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="63" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="62" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1672,7 +1672,7 @@
       <pane xSplit="3" ySplit="8" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1692,8 +1692,8 @@
       <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:38" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="66"/>
-      <c r="B2" s="66"/>
+      <c r="A2" s="85"/>
+      <c r="B2" s="85"/>
       <c r="C2" s="7"/>
       <c r="Y2" s="7"/>
       <c r="Z2" s="7"/>
@@ -1711,8 +1711,8 @@
       <c r="AL2" s="7"/>
     </row>
     <row r="3" spans="1:38" s="5" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A3" s="67"/>
-      <c r="B3" s="67"/>
+      <c r="A3" s="86"/>
+      <c r="B3" s="86"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -1752,165 +1752,165 @@
     </row>
     <row r="4" spans="1:38" s="4" customFormat="1" ht="15.75" thickBot="1"/>
     <row r="5" spans="1:38" ht="15" customHeight="1">
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="69"/>
-      <c r="D5" s="77" t="s">
+      <c r="C5" s="88"/>
+      <c r="D5" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="77" t="s">
+      <c r="E5" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="77" t="s">
+      <c r="F5" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="77" t="s">
+      <c r="G5" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="80" t="s">
+      <c r="H5" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="74" t="s">
+      <c r="I5" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="75"/>
-      <c r="K5" s="75"/>
-      <c r="L5" s="75"/>
-      <c r="M5" s="75"/>
-      <c r="N5" s="75"/>
-      <c r="O5" s="75"/>
-      <c r="P5" s="75"/>
-      <c r="Q5" s="75"/>
-      <c r="R5" s="75"/>
-      <c r="S5" s="75"/>
-      <c r="T5" s="75"/>
-      <c r="U5" s="75"/>
-      <c r="V5" s="75"/>
-      <c r="W5" s="75"/>
-      <c r="X5" s="75"/>
-      <c r="Y5" s="75"/>
-      <c r="Z5" s="75"/>
-      <c r="AA5" s="75"/>
-      <c r="AB5" s="75"/>
-      <c r="AC5" s="75"/>
-      <c r="AD5" s="75"/>
-      <c r="AE5" s="75"/>
-      <c r="AF5" s="75"/>
-      <c r="AG5" s="75"/>
-      <c r="AH5" s="75"/>
-      <c r="AI5" s="75"/>
-      <c r="AJ5" s="75"/>
-      <c r="AK5" s="75"/>
-      <c r="AL5" s="76"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="70"/>
+      <c r="M5" s="70"/>
+      <c r="N5" s="70"/>
+      <c r="O5" s="70"/>
+      <c r="P5" s="70"/>
+      <c r="Q5" s="70"/>
+      <c r="R5" s="70"/>
+      <c r="S5" s="70"/>
+      <c r="T5" s="70"/>
+      <c r="U5" s="70"/>
+      <c r="V5" s="70"/>
+      <c r="W5" s="70"/>
+      <c r="X5" s="70"/>
+      <c r="Y5" s="70"/>
+      <c r="Z5" s="70"/>
+      <c r="AA5" s="70"/>
+      <c r="AB5" s="70"/>
+      <c r="AC5" s="70"/>
+      <c r="AD5" s="70"/>
+      <c r="AE5" s="70"/>
+      <c r="AF5" s="70"/>
+      <c r="AG5" s="70"/>
+      <c r="AH5" s="70"/>
+      <c r="AI5" s="70"/>
+      <c r="AJ5" s="70"/>
+      <c r="AK5" s="70"/>
+      <c r="AL5" s="71"/>
     </row>
     <row r="6" spans="1:38">
-      <c r="B6" s="70"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="81"/>
-      <c r="I6" s="60">
+      <c r="B6" s="89"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
+      <c r="G6" s="73"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="59">
         <v>43892</v>
       </c>
-      <c r="J6" s="60">
+      <c r="J6" s="59">
         <v>43893</v>
       </c>
-      <c r="K6" s="60">
+      <c r="K6" s="59">
         <v>43894</v>
       </c>
-      <c r="L6" s="60">
+      <c r="L6" s="59">
         <v>43895</v>
       </c>
-      <c r="M6" s="60">
+      <c r="M6" s="59">
         <v>43896</v>
       </c>
-      <c r="N6" s="60">
+      <c r="N6" s="59">
         <v>43897</v>
       </c>
-      <c r="O6" s="60">
+      <c r="O6" s="59">
         <v>43898</v>
       </c>
-      <c r="P6" s="60">
+      <c r="P6" s="59">
         <v>43899</v>
       </c>
-      <c r="Q6" s="60">
+      <c r="Q6" s="59">
         <v>43900</v>
       </c>
-      <c r="R6" s="60">
+      <c r="R6" s="59">
         <v>43901</v>
       </c>
-      <c r="S6" s="60">
+      <c r="S6" s="59">
         <v>43902</v>
       </c>
-      <c r="T6" s="60">
+      <c r="T6" s="59">
         <v>43903</v>
       </c>
-      <c r="U6" s="60">
+      <c r="U6" s="59">
         <v>43904</v>
       </c>
-      <c r="V6" s="60">
+      <c r="V6" s="59">
         <v>43905</v>
       </c>
-      <c r="W6" s="60">
+      <c r="W6" s="59">
         <v>43906</v>
       </c>
-      <c r="X6" s="60">
+      <c r="X6" s="59">
         <v>43907</v>
       </c>
-      <c r="Y6" s="60">
+      <c r="Y6" s="59">
         <v>43908</v>
       </c>
-      <c r="Z6" s="60">
+      <c r="Z6" s="59">
         <v>43909</v>
       </c>
-      <c r="AA6" s="60">
+      <c r="AA6" s="59">
         <v>43910</v>
       </c>
-      <c r="AB6" s="60">
+      <c r="AB6" s="59">
         <v>43911</v>
       </c>
-      <c r="AC6" s="60">
+      <c r="AC6" s="59">
         <v>43912</v>
       </c>
-      <c r="AD6" s="60">
+      <c r="AD6" s="59">
         <v>43913</v>
       </c>
-      <c r="AE6" s="60">
+      <c r="AE6" s="59">
         <v>43914</v>
       </c>
-      <c r="AF6" s="60">
+      <c r="AF6" s="59">
         <v>43915</v>
       </c>
-      <c r="AG6" s="60">
+      <c r="AG6" s="59">
         <v>43916</v>
       </c>
-      <c r="AH6" s="60">
+      <c r="AH6" s="59">
         <v>43917</v>
       </c>
-      <c r="AI6" s="60">
+      <c r="AI6" s="59">
         <v>43918</v>
       </c>
-      <c r="AJ6" s="60">
+      <c r="AJ6" s="59">
         <v>43919</v>
       </c>
-      <c r="AK6" s="60">
+      <c r="AK6" s="59">
         <v>43920</v>
       </c>
-      <c r="AL6" s="57">
+      <c r="AL6" s="56">
         <v>43921</v>
       </c>
     </row>
     <row r="7" spans="1:38" ht="15.75" thickBot="1">
-      <c r="B7" s="72"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
-      <c r="G7" s="79"/>
-      <c r="H7" s="82"/>
+      <c r="B7" s="91"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="77"/>
       <c r="I7" s="1" t="str">
         <f>CHOOSE(WEEKDAY(I6),"日","月","火","水","木","金","土")</f>
         <v>月</v>
@@ -2034,306 +2034,308 @@
     </row>
     <row r="8" spans="1:38">
       <c r="A8" s="2"/>
-      <c r="B8" s="58"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="17"/>
-      <c r="R8" s="17"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="17"/>
-      <c r="U8" s="17"/>
-      <c r="V8" s="17"/>
-      <c r="W8" s="17"/>
-      <c r="X8" s="17"/>
-      <c r="Y8" s="17"/>
-      <c r="Z8" s="17"/>
-      <c r="AA8" s="17"/>
-      <c r="AB8" s="17"/>
-      <c r="AC8" s="17"/>
-      <c r="AD8" s="17"/>
-      <c r="AE8" s="17"/>
-      <c r="AF8" s="17"/>
-      <c r="AG8" s="17"/>
-      <c r="AH8" s="17"/>
-      <c r="AI8" s="17"/>
-      <c r="AJ8" s="17"/>
-      <c r="AK8" s="17"/>
-      <c r="AL8" s="18"/>
+      <c r="B8" s="57"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="16"/>
+      <c r="V8" s="16"/>
+      <c r="W8" s="16"/>
+      <c r="X8" s="16"/>
+      <c r="Y8" s="16"/>
+      <c r="Z8" s="16"/>
+      <c r="AA8" s="16"/>
+      <c r="AB8" s="16"/>
+      <c r="AC8" s="16"/>
+      <c r="AD8" s="16"/>
+      <c r="AE8" s="16"/>
+      <c r="AF8" s="16"/>
+      <c r="AG8" s="16"/>
+      <c r="AH8" s="16"/>
+      <c r="AI8" s="16"/>
+      <c r="AJ8" s="16"/>
+      <c r="AK8" s="16"/>
+      <c r="AL8" s="17"/>
     </row>
     <row r="9" spans="1:38" ht="26.25" customHeight="1">
       <c r="A9" s="2"/>
-      <c r="B9" s="62" t="s">
+      <c r="B9" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="21">
         <v>43892</v>
       </c>
-      <c r="E9" s="22">
+      <c r="E9" s="21">
         <v>43893</v>
       </c>
-      <c r="F9" s="22">
+      <c r="F9" s="21">
         <v>43892</v>
       </c>
-      <c r="G9" s="22">
+      <c r="G9" s="21">
         <v>43893</v>
       </c>
-      <c r="H9" s="61">
+      <c r="H9" s="60">
         <v>1</v>
       </c>
-      <c r="I9" s="40"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="41"/>
-      <c r="O9" s="41"/>
-      <c r="P9" s="41"/>
-      <c r="Q9" s="41"/>
-      <c r="R9" s="41"/>
-      <c r="S9" s="41"/>
-      <c r="T9" s="41"/>
-      <c r="U9" s="41"/>
-      <c r="V9" s="41"/>
-      <c r="W9" s="41"/>
-      <c r="X9" s="41"/>
-      <c r="Y9" s="41"/>
-      <c r="Z9" s="41"/>
-      <c r="AA9" s="41"/>
-      <c r="AB9" s="41"/>
-      <c r="AC9" s="41"/>
-      <c r="AD9" s="41"/>
-      <c r="AE9" s="41"/>
-      <c r="AF9" s="41"/>
-      <c r="AG9" s="41"/>
-      <c r="AH9" s="41"/>
-      <c r="AI9" s="41"/>
-      <c r="AJ9" s="41"/>
-      <c r="AK9" s="41"/>
-      <c r="AL9" s="42"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="40"/>
+      <c r="S9" s="40"/>
+      <c r="T9" s="40"/>
+      <c r="U9" s="40"/>
+      <c r="V9" s="40"/>
+      <c r="W9" s="40"/>
+      <c r="X9" s="40"/>
+      <c r="Y9" s="40"/>
+      <c r="Z9" s="40"/>
+      <c r="AA9" s="40"/>
+      <c r="AB9" s="40"/>
+      <c r="AC9" s="40"/>
+      <c r="AD9" s="40"/>
+      <c r="AE9" s="40"/>
+      <c r="AF9" s="40"/>
+      <c r="AG9" s="40"/>
+      <c r="AH9" s="40"/>
+      <c r="AI9" s="40"/>
+      <c r="AJ9" s="40"/>
+      <c r="AK9" s="40"/>
+      <c r="AL9" s="41"/>
     </row>
     <row r="10" spans="1:38" ht="26.25" customHeight="1">
       <c r="A10" s="2"/>
-      <c r="B10" s="62"/>
-      <c r="C10" s="86" t="s">
+      <c r="B10" s="78"/>
+      <c r="C10" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="87">
+      <c r="D10" s="62">
         <v>43892</v>
       </c>
-      <c r="E10" s="87">
+      <c r="E10" s="62">
         <v>43893</v>
       </c>
-      <c r="F10" s="87">
+      <c r="F10" s="62">
         <v>43892</v>
       </c>
-      <c r="G10" s="87">
+      <c r="G10" s="62">
         <v>43893</v>
       </c>
-      <c r="H10" s="88">
+      <c r="H10" s="63">
         <v>1</v>
       </c>
-      <c r="I10" s="49"/>
-      <c r="J10" s="50"/>
-      <c r="K10" s="50"/>
-      <c r="L10" s="50"/>
-      <c r="M10" s="50"/>
-      <c r="N10" s="50"/>
-      <c r="O10" s="50"/>
-      <c r="P10" s="50"/>
-      <c r="Q10" s="50"/>
-      <c r="R10" s="50"/>
-      <c r="S10" s="50"/>
-      <c r="T10" s="50"/>
-      <c r="U10" s="50"/>
-      <c r="V10" s="50"/>
-      <c r="W10" s="50"/>
-      <c r="X10" s="50"/>
-      <c r="Y10" s="50"/>
-      <c r="Z10" s="50"/>
-      <c r="AA10" s="50"/>
-      <c r="AB10" s="50"/>
-      <c r="AC10" s="50"/>
-      <c r="AD10" s="50"/>
-      <c r="AE10" s="50"/>
-      <c r="AF10" s="50"/>
-      <c r="AG10" s="50"/>
-      <c r="AH10" s="50"/>
-      <c r="AI10" s="50"/>
-      <c r="AJ10" s="50"/>
-      <c r="AK10" s="50"/>
-      <c r="AL10" s="51"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="49"/>
+      <c r="M10" s="49"/>
+      <c r="N10" s="49"/>
+      <c r="O10" s="49"/>
+      <c r="P10" s="49"/>
+      <c r="Q10" s="49"/>
+      <c r="R10" s="49"/>
+      <c r="S10" s="49"/>
+      <c r="T10" s="49"/>
+      <c r="U10" s="49"/>
+      <c r="V10" s="49"/>
+      <c r="W10" s="49"/>
+      <c r="X10" s="49"/>
+      <c r="Y10" s="49"/>
+      <c r="Z10" s="49"/>
+      <c r="AA10" s="49"/>
+      <c r="AB10" s="49"/>
+      <c r="AC10" s="49"/>
+      <c r="AD10" s="49"/>
+      <c r="AE10" s="49"/>
+      <c r="AF10" s="49"/>
+      <c r="AG10" s="49"/>
+      <c r="AH10" s="49"/>
+      <c r="AI10" s="49"/>
+      <c r="AJ10" s="49"/>
+      <c r="AK10" s="49"/>
+      <c r="AL10" s="50"/>
     </row>
     <row r="11" spans="1:38" ht="26.25" customHeight="1">
       <c r="A11" s="2"/>
-      <c r="B11" s="62"/>
-      <c r="C11" s="86" t="s">
+      <c r="B11" s="78"/>
+      <c r="C11" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="87">
+      <c r="D11" s="62">
         <v>43892</v>
       </c>
-      <c r="E11" s="87">
+      <c r="E11" s="62">
         <v>43893</v>
       </c>
-      <c r="F11" s="87">
+      <c r="F11" s="62">
         <v>43892</v>
       </c>
-      <c r="G11" s="87">
+      <c r="G11" s="62">
         <v>43893</v>
       </c>
-      <c r="H11" s="88">
+      <c r="H11" s="63">
         <v>1</v>
       </c>
-      <c r="I11" s="49"/>
-      <c r="J11" s="50"/>
-      <c r="K11" s="50"/>
-      <c r="L11" s="50"/>
-      <c r="M11" s="50"/>
-      <c r="N11" s="50"/>
-      <c r="O11" s="50"/>
-      <c r="P11" s="50"/>
-      <c r="Q11" s="50"/>
-      <c r="R11" s="50"/>
-      <c r="S11" s="50"/>
-      <c r="T11" s="50"/>
-      <c r="U11" s="50"/>
-      <c r="V11" s="50"/>
-      <c r="W11" s="50"/>
-      <c r="X11" s="50"/>
-      <c r="Y11" s="50"/>
-      <c r="Z11" s="50"/>
-      <c r="AA11" s="50"/>
-      <c r="AB11" s="50"/>
-      <c r="AC11" s="50"/>
-      <c r="AD11" s="50"/>
-      <c r="AE11" s="50"/>
-      <c r="AF11" s="50"/>
-      <c r="AG11" s="50"/>
-      <c r="AH11" s="50"/>
-      <c r="AI11" s="50"/>
-      <c r="AJ11" s="50"/>
-      <c r="AK11" s="50"/>
-      <c r="AL11" s="51"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="49"/>
+      <c r="L11" s="49"/>
+      <c r="M11" s="49"/>
+      <c r="N11" s="49"/>
+      <c r="O11" s="49"/>
+      <c r="P11" s="49"/>
+      <c r="Q11" s="49"/>
+      <c r="R11" s="49"/>
+      <c r="S11" s="49"/>
+      <c r="T11" s="49"/>
+      <c r="U11" s="49"/>
+      <c r="V11" s="49"/>
+      <c r="W11" s="49"/>
+      <c r="X11" s="49"/>
+      <c r="Y11" s="49"/>
+      <c r="Z11" s="49"/>
+      <c r="AA11" s="49"/>
+      <c r="AB11" s="49"/>
+      <c r="AC11" s="49"/>
+      <c r="AD11" s="49"/>
+      <c r="AE11" s="49"/>
+      <c r="AF11" s="49"/>
+      <c r="AG11" s="49"/>
+      <c r="AH11" s="49"/>
+      <c r="AI11" s="49"/>
+      <c r="AJ11" s="49"/>
+      <c r="AK11" s="49"/>
+      <c r="AL11" s="50"/>
     </row>
     <row r="12" spans="1:38" ht="26.25" customHeight="1">
       <c r="A12" s="2"/>
-      <c r="B12" s="62"/>
-      <c r="C12" s="86" t="s">
+      <c r="B12" s="78"/>
+      <c r="C12" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="87">
+      <c r="D12" s="62">
         <v>43892</v>
       </c>
-      <c r="E12" s="87">
+      <c r="E12" s="62">
         <v>43893</v>
       </c>
-      <c r="F12" s="87">
+      <c r="F12" s="62">
         <v>43892</v>
       </c>
-      <c r="G12" s="87">
+      <c r="G12" s="62">
         <v>43893</v>
       </c>
-      <c r="H12" s="88">
+      <c r="H12" s="63">
         <v>1</v>
       </c>
-      <c r="I12" s="49"/>
-      <c r="J12" s="50"/>
-      <c r="K12" s="50"/>
-      <c r="L12" s="50"/>
-      <c r="M12" s="50"/>
-      <c r="N12" s="50"/>
-      <c r="O12" s="50"/>
-      <c r="P12" s="50"/>
-      <c r="Q12" s="50"/>
-      <c r="R12" s="50"/>
-      <c r="S12" s="50"/>
-      <c r="T12" s="50"/>
-      <c r="U12" s="50"/>
-      <c r="V12" s="50"/>
-      <c r="W12" s="50"/>
-      <c r="X12" s="50"/>
-      <c r="Y12" s="50"/>
-      <c r="Z12" s="50"/>
-      <c r="AA12" s="50"/>
-      <c r="AB12" s="50"/>
-      <c r="AC12" s="50"/>
-      <c r="AD12" s="50"/>
-      <c r="AE12" s="50"/>
-      <c r="AF12" s="50"/>
-      <c r="AG12" s="50"/>
-      <c r="AH12" s="50"/>
-      <c r="AI12" s="50"/>
-      <c r="AJ12" s="50"/>
-      <c r="AK12" s="50"/>
-      <c r="AL12" s="51"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="49"/>
+      <c r="M12" s="49"/>
+      <c r="N12" s="49"/>
+      <c r="O12" s="49"/>
+      <c r="P12" s="49"/>
+      <c r="Q12" s="49"/>
+      <c r="R12" s="49"/>
+      <c r="S12" s="49"/>
+      <c r="T12" s="49"/>
+      <c r="U12" s="49"/>
+      <c r="V12" s="49"/>
+      <c r="W12" s="49"/>
+      <c r="X12" s="49"/>
+      <c r="Y12" s="49"/>
+      <c r="Z12" s="49"/>
+      <c r="AA12" s="49"/>
+      <c r="AB12" s="49"/>
+      <c r="AC12" s="49"/>
+      <c r="AD12" s="49"/>
+      <c r="AE12" s="49"/>
+      <c r="AF12" s="49"/>
+      <c r="AG12" s="49"/>
+      <c r="AH12" s="49"/>
+      <c r="AI12" s="49"/>
+      <c r="AJ12" s="49"/>
+      <c r="AK12" s="49"/>
+      <c r="AL12" s="50"/>
     </row>
     <row r="13" spans="1:38" ht="26.25" customHeight="1">
       <c r="A13" s="2"/>
-      <c r="B13" s="62"/>
-      <c r="C13" s="86" t="s">
+      <c r="B13" s="78"/>
+      <c r="C13" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="87">
+      <c r="D13" s="62">
         <v>43894</v>
       </c>
-      <c r="E13" s="87">
+      <c r="E13" s="62">
         <v>43895</v>
       </c>
-      <c r="F13" s="87">
+      <c r="F13" s="62">
         <v>43894</v>
       </c>
-      <c r="G13" s="87"/>
-      <c r="H13" s="88"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="50"/>
-      <c r="K13" s="50"/>
-      <c r="L13" s="50"/>
-      <c r="M13" s="50"/>
-      <c r="N13" s="50"/>
-      <c r="O13" s="50"/>
-      <c r="P13" s="50"/>
-      <c r="Q13" s="50"/>
-      <c r="R13" s="50"/>
-      <c r="S13" s="50"/>
-      <c r="T13" s="50"/>
-      <c r="U13" s="50"/>
-      <c r="V13" s="50"/>
-      <c r="W13" s="50"/>
-      <c r="X13" s="50"/>
-      <c r="Y13" s="50"/>
-      <c r="Z13" s="50"/>
-      <c r="AA13" s="50"/>
-      <c r="AB13" s="50"/>
-      <c r="AC13" s="50"/>
-      <c r="AD13" s="50"/>
-      <c r="AE13" s="50"/>
-      <c r="AF13" s="50"/>
-      <c r="AG13" s="50"/>
-      <c r="AH13" s="50"/>
-      <c r="AI13" s="50"/>
-      <c r="AJ13" s="50"/>
-      <c r="AK13" s="50"/>
-      <c r="AL13" s="51"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="63">
+        <v>0.9</v>
+      </c>
+      <c r="I13" s="48"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="49"/>
+      <c r="M13" s="49"/>
+      <c r="N13" s="49"/>
+      <c r="O13" s="49"/>
+      <c r="P13" s="49"/>
+      <c r="Q13" s="49"/>
+      <c r="R13" s="49"/>
+      <c r="S13" s="49"/>
+      <c r="T13" s="49"/>
+      <c r="U13" s="49"/>
+      <c r="V13" s="49"/>
+      <c r="W13" s="49"/>
+      <c r="X13" s="49"/>
+      <c r="Y13" s="49"/>
+      <c r="Z13" s="49"/>
+      <c r="AA13" s="49"/>
+      <c r="AB13" s="49"/>
+      <c r="AC13" s="49"/>
+      <c r="AD13" s="49"/>
+      <c r="AE13" s="49"/>
+      <c r="AF13" s="49"/>
+      <c r="AG13" s="49"/>
+      <c r="AH13" s="49"/>
+      <c r="AI13" s="49"/>
+      <c r="AJ13" s="49"/>
+      <c r="AK13" s="49"/>
+      <c r="AL13" s="50"/>
     </row>
     <row r="14" spans="1:38" ht="26.25" customHeight="1">
       <c r="A14" s="2"/>
-      <c r="B14" s="62"/>
-      <c r="C14" s="32" t="s">
+      <c r="B14" s="78"/>
+      <c r="C14" s="31" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="9">
@@ -2346,429 +2348,437 @@
         <v>43894</v>
       </c>
       <c r="G14" s="9"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="44"/>
-      <c r="K14" s="44"/>
-      <c r="L14" s="44"/>
-      <c r="M14" s="44"/>
-      <c r="N14" s="44"/>
-      <c r="O14" s="44"/>
-      <c r="P14" s="44"/>
-      <c r="Q14" s="44"/>
-      <c r="R14" s="44"/>
-      <c r="S14" s="44"/>
-      <c r="T14" s="44"/>
-      <c r="U14" s="44"/>
-      <c r="V14" s="44"/>
-      <c r="W14" s="44"/>
-      <c r="X14" s="44"/>
-      <c r="Y14" s="44"/>
-      <c r="Z14" s="44"/>
-      <c r="AA14" s="44"/>
-      <c r="AB14" s="44"/>
-      <c r="AC14" s="44"/>
-      <c r="AD14" s="44"/>
-      <c r="AE14" s="44"/>
-      <c r="AF14" s="44"/>
-      <c r="AG14" s="44"/>
-      <c r="AH14" s="44"/>
-      <c r="AI14" s="44"/>
-      <c r="AJ14" s="44"/>
-      <c r="AK14" s="44"/>
-      <c r="AL14" s="45"/>
+      <c r="H14" s="93">
+        <v>0.9</v>
+      </c>
+      <c r="I14" s="42"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="43"/>
+      <c r="Q14" s="43"/>
+      <c r="R14" s="43"/>
+      <c r="S14" s="43"/>
+      <c r="T14" s="43"/>
+      <c r="U14" s="43"/>
+      <c r="V14" s="43"/>
+      <c r="W14" s="43"/>
+      <c r="X14" s="43"/>
+      <c r="Y14" s="43"/>
+      <c r="Z14" s="43"/>
+      <c r="AA14" s="43"/>
+      <c r="AB14" s="43"/>
+      <c r="AC14" s="43"/>
+      <c r="AD14" s="43"/>
+      <c r="AE14" s="43"/>
+      <c r="AF14" s="43"/>
+      <c r="AG14" s="43"/>
+      <c r="AH14" s="43"/>
+      <c r="AI14" s="43"/>
+      <c r="AJ14" s="43"/>
+      <c r="AK14" s="43"/>
+      <c r="AL14" s="44"/>
     </row>
     <row r="15" spans="1:38" ht="26.25" customHeight="1">
       <c r="A15" s="2"/>
-      <c r="B15" s="62"/>
-      <c r="C15" s="89" t="s">
+      <c r="B15" s="78"/>
+      <c r="C15" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="90">
+      <c r="D15" s="65">
         <v>43895</v>
       </c>
-      <c r="E15" s="90">
+      <c r="E15" s="65">
         <v>43896</v>
       </c>
-      <c r="F15" s="90">
+      <c r="F15" s="65">
         <v>43894</v>
       </c>
-      <c r="G15" s="90"/>
-      <c r="H15" s="91"/>
-      <c r="I15" s="92"/>
-      <c r="J15" s="93"/>
-      <c r="K15" s="93"/>
-      <c r="L15" s="93"/>
-      <c r="M15" s="93"/>
-      <c r="N15" s="93"/>
-      <c r="O15" s="93"/>
-      <c r="P15" s="93"/>
-      <c r="Q15" s="93"/>
-      <c r="R15" s="93"/>
-      <c r="S15" s="93"/>
-      <c r="T15" s="93"/>
-      <c r="U15" s="93"/>
-      <c r="V15" s="93"/>
-      <c r="W15" s="93"/>
-      <c r="X15" s="93"/>
-      <c r="Y15" s="93"/>
-      <c r="Z15" s="93"/>
-      <c r="AA15" s="93"/>
-      <c r="AB15" s="93"/>
-      <c r="AC15" s="93"/>
-      <c r="AD15" s="93"/>
-      <c r="AE15" s="93"/>
-      <c r="AF15" s="93"/>
-      <c r="AG15" s="93"/>
-      <c r="AH15" s="93"/>
-      <c r="AI15" s="93"/>
-      <c r="AJ15" s="93"/>
-      <c r="AK15" s="93"/>
-      <c r="AL15" s="94"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="94">
+        <v>0.9</v>
+      </c>
+      <c r="I15" s="66"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="67"/>
+      <c r="L15" s="67"/>
+      <c r="M15" s="67"/>
+      <c r="N15" s="67"/>
+      <c r="O15" s="67"/>
+      <c r="P15" s="67"/>
+      <c r="Q15" s="67"/>
+      <c r="R15" s="67"/>
+      <c r="S15" s="67"/>
+      <c r="T15" s="67"/>
+      <c r="U15" s="67"/>
+      <c r="V15" s="67"/>
+      <c r="W15" s="67"/>
+      <c r="X15" s="67"/>
+      <c r="Y15" s="67"/>
+      <c r="Z15" s="67"/>
+      <c r="AA15" s="67"/>
+      <c r="AB15" s="67"/>
+      <c r="AC15" s="67"/>
+      <c r="AD15" s="67"/>
+      <c r="AE15" s="67"/>
+      <c r="AF15" s="67"/>
+      <c r="AG15" s="67"/>
+      <c r="AH15" s="67"/>
+      <c r="AI15" s="67"/>
+      <c r="AJ15" s="67"/>
+      <c r="AK15" s="67"/>
+      <c r="AL15" s="68"/>
     </row>
     <row r="16" spans="1:38" ht="26.25" customHeight="1">
       <c r="A16" s="2"/>
-      <c r="B16" s="62"/>
-      <c r="C16" s="89" t="s">
+      <c r="B16" s="78"/>
+      <c r="C16" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="90">
+      <c r="D16" s="65">
         <v>43895</v>
       </c>
-      <c r="E16" s="90">
+      <c r="E16" s="65">
         <v>43896</v>
       </c>
-      <c r="F16" s="90"/>
-      <c r="G16" s="90"/>
-      <c r="H16" s="91"/>
-      <c r="I16" s="92"/>
-      <c r="J16" s="93"/>
-      <c r="K16" s="93"/>
-      <c r="L16" s="93"/>
-      <c r="M16" s="93"/>
-      <c r="N16" s="93"/>
-      <c r="O16" s="93"/>
-      <c r="P16" s="93"/>
-      <c r="Q16" s="93"/>
-      <c r="R16" s="93"/>
-      <c r="S16" s="93"/>
-      <c r="T16" s="93"/>
-      <c r="U16" s="93"/>
-      <c r="V16" s="93"/>
-      <c r="W16" s="93"/>
-      <c r="X16" s="93"/>
-      <c r="Y16" s="93"/>
-      <c r="Z16" s="93"/>
-      <c r="AA16" s="93"/>
-      <c r="AB16" s="93"/>
-      <c r="AC16" s="93"/>
-      <c r="AD16" s="93"/>
-      <c r="AE16" s="93"/>
-      <c r="AF16" s="93"/>
-      <c r="AG16" s="93"/>
-      <c r="AH16" s="93"/>
-      <c r="AI16" s="93"/>
-      <c r="AJ16" s="93"/>
-      <c r="AK16" s="93"/>
-      <c r="AL16" s="94"/>
+      <c r="F16" s="65">
+        <v>43895</v>
+      </c>
+      <c r="G16" s="65"/>
+      <c r="H16" s="94">
+        <v>0.9</v>
+      </c>
+      <c r="I16" s="66"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="67"/>
+      <c r="M16" s="67"/>
+      <c r="N16" s="67"/>
+      <c r="O16" s="67"/>
+      <c r="P16" s="67"/>
+      <c r="Q16" s="67"/>
+      <c r="R16" s="67"/>
+      <c r="S16" s="67"/>
+      <c r="T16" s="67"/>
+      <c r="U16" s="67"/>
+      <c r="V16" s="67"/>
+      <c r="W16" s="67"/>
+      <c r="X16" s="67"/>
+      <c r="Y16" s="67"/>
+      <c r="Z16" s="67"/>
+      <c r="AA16" s="67"/>
+      <c r="AB16" s="67"/>
+      <c r="AC16" s="67"/>
+      <c r="AD16" s="67"/>
+      <c r="AE16" s="67"/>
+      <c r="AF16" s="67"/>
+      <c r="AG16" s="67"/>
+      <c r="AH16" s="67"/>
+      <c r="AI16" s="67"/>
+      <c r="AJ16" s="67"/>
+      <c r="AK16" s="67"/>
+      <c r="AL16" s="68"/>
     </row>
     <row r="17" spans="1:38" ht="26.25" customHeight="1">
       <c r="A17" s="2"/>
-      <c r="B17" s="62"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="47"/>
-      <c r="K17" s="47"/>
-      <c r="L17" s="47"/>
-      <c r="M17" s="47"/>
-      <c r="N17" s="47"/>
-      <c r="O17" s="47"/>
-      <c r="P17" s="47"/>
-      <c r="Q17" s="47"/>
-      <c r="R17" s="47"/>
-      <c r="S17" s="47"/>
-      <c r="T17" s="47"/>
-      <c r="U17" s="47"/>
-      <c r="V17" s="47"/>
-      <c r="W17" s="47"/>
-      <c r="X17" s="47"/>
-      <c r="Y17" s="47"/>
-      <c r="Z17" s="47"/>
-      <c r="AA17" s="47"/>
-      <c r="AB17" s="47"/>
-      <c r="AC17" s="47"/>
-      <c r="AD17" s="47"/>
-      <c r="AE17" s="47"/>
-      <c r="AF17" s="47"/>
-      <c r="AG17" s="47"/>
-      <c r="AH17" s="47"/>
-      <c r="AI17" s="47"/>
-      <c r="AJ17" s="47"/>
-      <c r="AK17" s="47"/>
-      <c r="AL17" s="48"/>
+      <c r="B17" s="78"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="46"/>
+      <c r="N17" s="46"/>
+      <c r="O17" s="46"/>
+      <c r="P17" s="46"/>
+      <c r="Q17" s="46"/>
+      <c r="R17" s="46"/>
+      <c r="S17" s="46"/>
+      <c r="T17" s="46"/>
+      <c r="U17" s="46"/>
+      <c r="V17" s="46"/>
+      <c r="W17" s="46"/>
+      <c r="X17" s="46"/>
+      <c r="Y17" s="46"/>
+      <c r="Z17" s="46"/>
+      <c r="AA17" s="46"/>
+      <c r="AB17" s="46"/>
+      <c r="AC17" s="46"/>
+      <c r="AD17" s="46"/>
+      <c r="AE17" s="46"/>
+      <c r="AF17" s="46"/>
+      <c r="AG17" s="46"/>
+      <c r="AH17" s="46"/>
+      <c r="AI17" s="46"/>
+      <c r="AJ17" s="46"/>
+      <c r="AK17" s="46"/>
+      <c r="AL17" s="47"/>
     </row>
     <row r="18" spans="1:38" ht="26.25" customHeight="1">
       <c r="A18" s="2"/>
-      <c r="B18" s="83" t="s">
+      <c r="B18" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="41"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="41"/>
-      <c r="N18" s="41"/>
-      <c r="O18" s="41"/>
-      <c r="P18" s="41"/>
-      <c r="Q18" s="41"/>
-      <c r="R18" s="41"/>
-      <c r="S18" s="41"/>
-      <c r="T18" s="41"/>
-      <c r="U18" s="41"/>
-      <c r="V18" s="41"/>
-      <c r="W18" s="41"/>
-      <c r="X18" s="41"/>
-      <c r="Y18" s="41"/>
-      <c r="Z18" s="41"/>
-      <c r="AA18" s="41"/>
-      <c r="AB18" s="41"/>
-      <c r="AC18" s="41"/>
-      <c r="AD18" s="41"/>
-      <c r="AE18" s="41"/>
-      <c r="AF18" s="41"/>
-      <c r="AG18" s="41"/>
-      <c r="AH18" s="41"/>
-      <c r="AI18" s="41"/>
-      <c r="AJ18" s="41"/>
-      <c r="AK18" s="41"/>
-      <c r="AL18" s="42"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="40"/>
+      <c r="O18" s="40"/>
+      <c r="P18" s="40"/>
+      <c r="Q18" s="40"/>
+      <c r="R18" s="40"/>
+      <c r="S18" s="40"/>
+      <c r="T18" s="40"/>
+      <c r="U18" s="40"/>
+      <c r="V18" s="40"/>
+      <c r="W18" s="40"/>
+      <c r="X18" s="40"/>
+      <c r="Y18" s="40"/>
+      <c r="Z18" s="40"/>
+      <c r="AA18" s="40"/>
+      <c r="AB18" s="40"/>
+      <c r="AC18" s="40"/>
+      <c r="AD18" s="40"/>
+      <c r="AE18" s="40"/>
+      <c r="AF18" s="40"/>
+      <c r="AG18" s="40"/>
+      <c r="AH18" s="40"/>
+      <c r="AI18" s="40"/>
+      <c r="AJ18" s="40"/>
+      <c r="AK18" s="40"/>
+      <c r="AL18" s="41"/>
     </row>
     <row r="19" spans="1:38" ht="26.25" customHeight="1">
       <c r="A19" s="2"/>
-      <c r="B19" s="84"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
-      <c r="K19" s="44"/>
-      <c r="L19" s="44"/>
-      <c r="M19" s="44"/>
-      <c r="N19" s="44"/>
-      <c r="O19" s="44"/>
-      <c r="P19" s="44"/>
-      <c r="Q19" s="44"/>
-      <c r="R19" s="44"/>
-      <c r="S19" s="44"/>
-      <c r="T19" s="44"/>
-      <c r="U19" s="44"/>
-      <c r="V19" s="44"/>
-      <c r="W19" s="44"/>
-      <c r="X19" s="44"/>
-      <c r="Y19" s="44"/>
-      <c r="Z19" s="44"/>
-      <c r="AA19" s="44"/>
-      <c r="AB19" s="44"/>
-      <c r="AC19" s="44"/>
-      <c r="AD19" s="44"/>
-      <c r="AE19" s="44"/>
-      <c r="AF19" s="44"/>
-      <c r="AG19" s="44"/>
-      <c r="AH19" s="44"/>
-      <c r="AI19" s="44"/>
-      <c r="AJ19" s="44"/>
-      <c r="AK19" s="44"/>
-      <c r="AL19" s="45"/>
+      <c r="B19" s="80"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="43"/>
+      <c r="O19" s="43"/>
+      <c r="P19" s="43"/>
+      <c r="Q19" s="43"/>
+      <c r="R19" s="43"/>
+      <c r="S19" s="43"/>
+      <c r="T19" s="43"/>
+      <c r="U19" s="43"/>
+      <c r="V19" s="43"/>
+      <c r="W19" s="43"/>
+      <c r="X19" s="43"/>
+      <c r="Y19" s="43"/>
+      <c r="Z19" s="43"/>
+      <c r="AA19" s="43"/>
+      <c r="AB19" s="43"/>
+      <c r="AC19" s="43"/>
+      <c r="AD19" s="43"/>
+      <c r="AE19" s="43"/>
+      <c r="AF19" s="43"/>
+      <c r="AG19" s="43"/>
+      <c r="AH19" s="43"/>
+      <c r="AI19" s="43"/>
+      <c r="AJ19" s="43"/>
+      <c r="AK19" s="43"/>
+      <c r="AL19" s="44"/>
     </row>
     <row r="20" spans="1:38" ht="26.25" customHeight="1">
       <c r="A20" s="2"/>
-      <c r="B20" s="85"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="47"/>
-      <c r="J20" s="47"/>
-      <c r="K20" s="47"/>
-      <c r="L20" s="47"/>
-      <c r="M20" s="47"/>
-      <c r="N20" s="47"/>
-      <c r="O20" s="47"/>
-      <c r="P20" s="47"/>
-      <c r="Q20" s="47"/>
-      <c r="R20" s="47"/>
-      <c r="S20" s="47"/>
-      <c r="T20" s="47"/>
-      <c r="U20" s="47"/>
-      <c r="V20" s="47"/>
-      <c r="W20" s="47"/>
-      <c r="X20" s="47"/>
-      <c r="Y20" s="47"/>
-      <c r="Z20" s="47"/>
-      <c r="AA20" s="47"/>
-      <c r="AB20" s="47"/>
-      <c r="AC20" s="47"/>
-      <c r="AD20" s="47"/>
-      <c r="AE20" s="47"/>
-      <c r="AF20" s="47"/>
-      <c r="AG20" s="47"/>
-      <c r="AH20" s="47"/>
-      <c r="AI20" s="47"/>
-      <c r="AJ20" s="47"/>
-      <c r="AK20" s="47"/>
-      <c r="AL20" s="48"/>
+      <c r="B20" s="81"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="46"/>
+      <c r="L20" s="46"/>
+      <c r="M20" s="46"/>
+      <c r="N20" s="46"/>
+      <c r="O20" s="46"/>
+      <c r="P20" s="46"/>
+      <c r="Q20" s="46"/>
+      <c r="R20" s="46"/>
+      <c r="S20" s="46"/>
+      <c r="T20" s="46"/>
+      <c r="U20" s="46"/>
+      <c r="V20" s="46"/>
+      <c r="W20" s="46"/>
+      <c r="X20" s="46"/>
+      <c r="Y20" s="46"/>
+      <c r="Z20" s="46"/>
+      <c r="AA20" s="46"/>
+      <c r="AB20" s="46"/>
+      <c r="AC20" s="46"/>
+      <c r="AD20" s="46"/>
+      <c r="AE20" s="46"/>
+      <c r="AF20" s="46"/>
+      <c r="AG20" s="46"/>
+      <c r="AH20" s="46"/>
+      <c r="AI20" s="46"/>
+      <c r="AJ20" s="46"/>
+      <c r="AK20" s="46"/>
+      <c r="AL20" s="47"/>
     </row>
     <row r="21" spans="1:38" ht="26.25" customHeight="1">
-      <c r="A21" s="15"/>
-      <c r="B21" s="63" t="s">
+      <c r="A21" s="14"/>
+      <c r="B21" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="37"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="49"/>
-      <c r="J21" s="50"/>
-      <c r="K21" s="50"/>
-      <c r="L21" s="50"/>
-      <c r="M21" s="50"/>
-      <c r="N21" s="50"/>
-      <c r="O21" s="50"/>
-      <c r="P21" s="50"/>
-      <c r="Q21" s="50"/>
-      <c r="R21" s="50"/>
-      <c r="S21" s="50"/>
-      <c r="T21" s="50"/>
-      <c r="U21" s="50"/>
-      <c r="V21" s="50"/>
-      <c r="W21" s="50"/>
-      <c r="X21" s="50"/>
-      <c r="Y21" s="50"/>
-      <c r="Z21" s="50"/>
-      <c r="AA21" s="50"/>
-      <c r="AB21" s="50"/>
-      <c r="AC21" s="50"/>
-      <c r="AD21" s="50"/>
-      <c r="AE21" s="50"/>
-      <c r="AF21" s="50"/>
-      <c r="AG21" s="50"/>
-      <c r="AH21" s="50"/>
-      <c r="AI21" s="50"/>
-      <c r="AJ21" s="50"/>
-      <c r="AK21" s="50"/>
-      <c r="AL21" s="51"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="49"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="49"/>
+      <c r="N21" s="49"/>
+      <c r="O21" s="49"/>
+      <c r="P21" s="49"/>
+      <c r="Q21" s="49"/>
+      <c r="R21" s="49"/>
+      <c r="S21" s="49"/>
+      <c r="T21" s="49"/>
+      <c r="U21" s="49"/>
+      <c r="V21" s="49"/>
+      <c r="W21" s="49"/>
+      <c r="X21" s="49"/>
+      <c r="Y21" s="49"/>
+      <c r="Z21" s="49"/>
+      <c r="AA21" s="49"/>
+      <c r="AB21" s="49"/>
+      <c r="AC21" s="49"/>
+      <c r="AD21" s="49"/>
+      <c r="AE21" s="49"/>
+      <c r="AF21" s="49"/>
+      <c r="AG21" s="49"/>
+      <c r="AH21" s="49"/>
+      <c r="AI21" s="49"/>
+      <c r="AJ21" s="49"/>
+      <c r="AK21" s="49"/>
+      <c r="AL21" s="50"/>
     </row>
     <row r="22" spans="1:38" ht="26.25" customHeight="1">
-      <c r="A22" s="15"/>
-      <c r="B22" s="64"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="44"/>
-      <c r="K22" s="52"/>
-      <c r="L22" s="52"/>
-      <c r="M22" s="52"/>
-      <c r="N22" s="52"/>
-      <c r="O22" s="44"/>
-      <c r="P22" s="44"/>
-      <c r="Q22" s="52"/>
-      <c r="R22" s="52"/>
-      <c r="S22" s="52"/>
-      <c r="T22" s="52"/>
-      <c r="U22" s="52"/>
-      <c r="V22" s="44"/>
-      <c r="W22" s="44"/>
-      <c r="X22" s="52"/>
-      <c r="Y22" s="52"/>
-      <c r="Z22" s="52"/>
-      <c r="AA22" s="52"/>
-      <c r="AB22" s="52"/>
-      <c r="AC22" s="44"/>
-      <c r="AD22" s="44"/>
-      <c r="AE22" s="52"/>
-      <c r="AF22" s="52"/>
-      <c r="AG22" s="52"/>
-      <c r="AH22" s="52"/>
-      <c r="AI22" s="52"/>
-      <c r="AJ22" s="44"/>
-      <c r="AK22" s="44"/>
-      <c r="AL22" s="53"/>
+      <c r="A22" s="14"/>
+      <c r="B22" s="83"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="51"/>
+      <c r="L22" s="51"/>
+      <c r="M22" s="51"/>
+      <c r="N22" s="51"/>
+      <c r="O22" s="43"/>
+      <c r="P22" s="43"/>
+      <c r="Q22" s="51"/>
+      <c r="R22" s="51"/>
+      <c r="S22" s="51"/>
+      <c r="T22" s="51"/>
+      <c r="U22" s="51"/>
+      <c r="V22" s="43"/>
+      <c r="W22" s="43"/>
+      <c r="X22" s="51"/>
+      <c r="Y22" s="51"/>
+      <c r="Z22" s="51"/>
+      <c r="AA22" s="51"/>
+      <c r="AB22" s="51"/>
+      <c r="AC22" s="43"/>
+      <c r="AD22" s="43"/>
+      <c r="AE22" s="51"/>
+      <c r="AF22" s="51"/>
+      <c r="AG22" s="51"/>
+      <c r="AH22" s="51"/>
+      <c r="AI22" s="51"/>
+      <c r="AJ22" s="43"/>
+      <c r="AK22" s="43"/>
+      <c r="AL22" s="52"/>
     </row>
     <row r="23" spans="1:38" ht="26.25" customHeight="1" thickBot="1">
-      <c r="A23" s="15"/>
-      <c r="B23" s="65"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="55"/>
-      <c r="L23" s="55"/>
-      <c r="M23" s="55"/>
-      <c r="N23" s="55"/>
-      <c r="O23" s="54"/>
-      <c r="P23" s="54"/>
-      <c r="Q23" s="55"/>
-      <c r="R23" s="55"/>
-      <c r="S23" s="55"/>
-      <c r="T23" s="55"/>
-      <c r="U23" s="55"/>
-      <c r="V23" s="54"/>
-      <c r="W23" s="54"/>
-      <c r="X23" s="55"/>
-      <c r="Y23" s="55"/>
-      <c r="Z23" s="55"/>
-      <c r="AA23" s="55"/>
-      <c r="AB23" s="55"/>
-      <c r="AC23" s="54"/>
-      <c r="AD23" s="54"/>
-      <c r="AE23" s="55"/>
-      <c r="AF23" s="55"/>
-      <c r="AG23" s="55"/>
-      <c r="AH23" s="55"/>
-      <c r="AI23" s="55"/>
-      <c r="AJ23" s="54"/>
-      <c r="AK23" s="54"/>
-      <c r="AL23" s="56"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="84"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="53"/>
+      <c r="K23" s="54"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="54"/>
+      <c r="N23" s="54"/>
+      <c r="O23" s="53"/>
+      <c r="P23" s="53"/>
+      <c r="Q23" s="54"/>
+      <c r="R23" s="54"/>
+      <c r="S23" s="54"/>
+      <c r="T23" s="54"/>
+      <c r="U23" s="54"/>
+      <c r="V23" s="53"/>
+      <c r="W23" s="53"/>
+      <c r="X23" s="54"/>
+      <c r="Y23" s="54"/>
+      <c r="Z23" s="54"/>
+      <c r="AA23" s="54"/>
+      <c r="AB23" s="54"/>
+      <c r="AC23" s="53"/>
+      <c r="AD23" s="53"/>
+      <c r="AE23" s="54"/>
+      <c r="AF23" s="54"/>
+      <c r="AG23" s="54"/>
+      <c r="AH23" s="54"/>
+      <c r="AI23" s="54"/>
+      <c r="AJ23" s="53"/>
+      <c r="AK23" s="53"/>
+      <c r="AL23" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B9:B17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="B5:C7"/>
     <mergeCell ref="I5:AL5"/>
     <mergeCell ref="D5:D7"/>
     <mergeCell ref="E5:E7"/>
     <mergeCell ref="F5:F7"/>
     <mergeCell ref="G5:G7"/>
     <mergeCell ref="H5:H7"/>
-    <mergeCell ref="B9:B17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="B5:C7"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="H21:H23 H9:H16">

</xml_diff>

<commit_message>
Commit code ngày 2020/03/06
</commit_message>
<xml_diff>
--- a/Document/Schedule.xlsx
+++ b/Document/Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QuyenNQ\Documents\Trainning202003\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6EFDAD-F9E3-498F-B7BD-A22FB86980D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DABDBD5-57E0-4CBB-9BBF-382346102570}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="1035" windowWidth="21600" windowHeight="14085" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3465" yWindow="1380" windowWidth="21600" windowHeight="14085" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Schedule" sheetId="2" r:id="rId1"/>
@@ -1221,6 +1221,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="4" borderId="62" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1246,57 +1297,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="4" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="4" borderId="62" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1672,7 +1672,7 @@
       <pane xSplit="3" ySplit="8" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1692,8 +1692,8 @@
       <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:38" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="A2" s="85"/>
-      <c r="B2" s="85"/>
+      <c r="A2" s="78"/>
+      <c r="B2" s="78"/>
       <c r="C2" s="7"/>
       <c r="Y2" s="7"/>
       <c r="Z2" s="7"/>
@@ -1711,8 +1711,8 @@
       <c r="AL2" s="7"/>
     </row>
     <row r="3" spans="1:38" s="5" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A3" s="86"/>
-      <c r="B3" s="86"/>
+      <c r="A3" s="79"/>
+      <c r="B3" s="79"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -1752,66 +1752,66 @@
     </row>
     <row r="4" spans="1:38" s="4" customFormat="1" ht="15.75" thickBot="1"/>
     <row r="5" spans="1:38" ht="15" customHeight="1">
-      <c r="B5" s="87" t="s">
+      <c r="B5" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="88"/>
-      <c r="D5" s="72" t="s">
+      <c r="C5" s="81"/>
+      <c r="D5" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="72" t="s">
+      <c r="E5" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="72" t="s">
+      <c r="F5" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="72" t="s">
+      <c r="G5" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="75" t="s">
+      <c r="H5" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="69" t="s">
+      <c r="I5" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="70"/>
-      <c r="K5" s="70"/>
-      <c r="L5" s="70"/>
-      <c r="M5" s="70"/>
-      <c r="N5" s="70"/>
-      <c r="O5" s="70"/>
-      <c r="P5" s="70"/>
-      <c r="Q5" s="70"/>
-      <c r="R5" s="70"/>
-      <c r="S5" s="70"/>
-      <c r="T5" s="70"/>
-      <c r="U5" s="70"/>
-      <c r="V5" s="70"/>
-      <c r="W5" s="70"/>
-      <c r="X5" s="70"/>
-      <c r="Y5" s="70"/>
-      <c r="Z5" s="70"/>
-      <c r="AA5" s="70"/>
-      <c r="AB5" s="70"/>
-      <c r="AC5" s="70"/>
-      <c r="AD5" s="70"/>
-      <c r="AE5" s="70"/>
-      <c r="AF5" s="70"/>
-      <c r="AG5" s="70"/>
-      <c r="AH5" s="70"/>
-      <c r="AI5" s="70"/>
-      <c r="AJ5" s="70"/>
-      <c r="AK5" s="70"/>
-      <c r="AL5" s="71"/>
+      <c r="J5" s="87"/>
+      <c r="K5" s="87"/>
+      <c r="L5" s="87"/>
+      <c r="M5" s="87"/>
+      <c r="N5" s="87"/>
+      <c r="O5" s="87"/>
+      <c r="P5" s="87"/>
+      <c r="Q5" s="87"/>
+      <c r="R5" s="87"/>
+      <c r="S5" s="87"/>
+      <c r="T5" s="87"/>
+      <c r="U5" s="87"/>
+      <c r="V5" s="87"/>
+      <c r="W5" s="87"/>
+      <c r="X5" s="87"/>
+      <c r="Y5" s="87"/>
+      <c r="Z5" s="87"/>
+      <c r="AA5" s="87"/>
+      <c r="AB5" s="87"/>
+      <c r="AC5" s="87"/>
+      <c r="AD5" s="87"/>
+      <c r="AE5" s="87"/>
+      <c r="AF5" s="87"/>
+      <c r="AG5" s="87"/>
+      <c r="AH5" s="87"/>
+      <c r="AI5" s="87"/>
+      <c r="AJ5" s="87"/>
+      <c r="AK5" s="87"/>
+      <c r="AL5" s="88"/>
     </row>
     <row r="6" spans="1:38">
-      <c r="B6" s="89"/>
-      <c r="C6" s="90"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="76"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="90"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="90"/>
+      <c r="H6" s="93"/>
       <c r="I6" s="59">
         <v>43892</v>
       </c>
@@ -1904,13 +1904,13 @@
       </c>
     </row>
     <row r="7" spans="1:38" ht="15.75" thickBot="1">
-      <c r="B7" s="91"/>
-      <c r="C7" s="92"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="77"/>
+      <c r="B7" s="84"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="91"/>
+      <c r="E7" s="91"/>
+      <c r="F7" s="91"/>
+      <c r="G7" s="91"/>
+      <c r="H7" s="94"/>
       <c r="I7" s="1" t="str">
         <f>CHOOSE(WEEKDAY(I6),"日","月","火","水","木","金","土")</f>
         <v>月</v>
@@ -2074,7 +2074,7 @@
     </row>
     <row r="9" spans="1:38" ht="26.25" customHeight="1">
       <c r="A9" s="2"/>
-      <c r="B9" s="78" t="s">
+      <c r="B9" s="71" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="30" t="s">
@@ -2128,7 +2128,7 @@
     </row>
     <row r="10" spans="1:38" ht="26.25" customHeight="1">
       <c r="A10" s="2"/>
-      <c r="B10" s="78"/>
+      <c r="B10" s="71"/>
       <c r="C10" s="61" t="s">
         <v>12</v>
       </c>
@@ -2180,7 +2180,7 @@
     </row>
     <row r="11" spans="1:38" ht="26.25" customHeight="1">
       <c r="A11" s="2"/>
-      <c r="B11" s="78"/>
+      <c r="B11" s="71"/>
       <c r="C11" s="61" t="s">
         <v>11</v>
       </c>
@@ -2232,7 +2232,7 @@
     </row>
     <row r="12" spans="1:38" ht="26.25" customHeight="1">
       <c r="A12" s="2"/>
-      <c r="B12" s="78"/>
+      <c r="B12" s="71"/>
       <c r="C12" s="61" t="s">
         <v>10</v>
       </c>
@@ -2284,7 +2284,7 @@
     </row>
     <row r="13" spans="1:38" ht="26.25" customHeight="1">
       <c r="A13" s="2"/>
-      <c r="B13" s="78"/>
+      <c r="B13" s="71"/>
       <c r="C13" s="61" t="s">
         <v>14</v>
       </c>
@@ -2297,9 +2297,11 @@
       <c r="F13" s="62">
         <v>43894</v>
       </c>
-      <c r="G13" s="62"/>
+      <c r="G13" s="62">
+        <v>43896</v>
+      </c>
       <c r="H13" s="63">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="I13" s="48"/>
       <c r="J13" s="49"/>
@@ -2334,7 +2336,7 @@
     </row>
     <row r="14" spans="1:38" ht="26.25" customHeight="1">
       <c r="A14" s="2"/>
-      <c r="B14" s="78"/>
+      <c r="B14" s="71"/>
       <c r="C14" s="31" t="s">
         <v>17</v>
       </c>
@@ -2347,9 +2349,11 @@
       <c r="F14" s="9">
         <v>43894</v>
       </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="93">
-        <v>0.9</v>
+      <c r="G14" s="9">
+        <v>43896</v>
+      </c>
+      <c r="H14" s="69">
+        <v>1</v>
       </c>
       <c r="I14" s="42"/>
       <c r="J14" s="43"/>
@@ -2384,7 +2388,7 @@
     </row>
     <row r="15" spans="1:38" ht="26.25" customHeight="1">
       <c r="A15" s="2"/>
-      <c r="B15" s="78"/>
+      <c r="B15" s="71"/>
       <c r="C15" s="64" t="s">
         <v>16</v>
       </c>
@@ -2397,9 +2401,11 @@
       <c r="F15" s="65">
         <v>43894</v>
       </c>
-      <c r="G15" s="65"/>
-      <c r="H15" s="94">
-        <v>0.9</v>
+      <c r="G15" s="65">
+        <v>43896</v>
+      </c>
+      <c r="H15" s="70">
+        <v>1</v>
       </c>
       <c r="I15" s="66"/>
       <c r="J15" s="67"/>
@@ -2434,7 +2440,7 @@
     </row>
     <row r="16" spans="1:38" ht="26.25" customHeight="1">
       <c r="A16" s="2"/>
-      <c r="B16" s="78"/>
+      <c r="B16" s="71"/>
       <c r="C16" s="64" t="s">
         <v>15</v>
       </c>
@@ -2447,9 +2453,11 @@
       <c r="F16" s="65">
         <v>43895</v>
       </c>
-      <c r="G16" s="65"/>
-      <c r="H16" s="94">
-        <v>0.9</v>
+      <c r="G16" s="65">
+        <v>43896</v>
+      </c>
+      <c r="H16" s="70">
+        <v>1</v>
       </c>
       <c r="I16" s="66"/>
       <c r="J16" s="67"/>
@@ -2484,7 +2492,7 @@
     </row>
     <row r="17" spans="1:38" ht="26.25" customHeight="1">
       <c r="A17" s="2"/>
-      <c r="B17" s="78"/>
+      <c r="B17" s="71"/>
       <c r="C17" s="32"/>
       <c r="D17" s="22"/>
       <c r="E17" s="22"/>
@@ -2524,7 +2532,7 @@
     </row>
     <row r="18" spans="1:38" ht="26.25" customHeight="1">
       <c r="A18" s="2"/>
-      <c r="B18" s="79" t="s">
+      <c r="B18" s="72" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="33"/>
@@ -2566,7 +2574,7 @@
     </row>
     <row r="19" spans="1:38" ht="26.25" customHeight="1">
       <c r="A19" s="2"/>
-      <c r="B19" s="80"/>
+      <c r="B19" s="73"/>
       <c r="C19" s="34"/>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
@@ -2606,7 +2614,7 @@
     </row>
     <row r="20" spans="1:38" ht="26.25" customHeight="1">
       <c r="A20" s="2"/>
-      <c r="B20" s="81"/>
+      <c r="B20" s="74"/>
       <c r="C20" s="35"/>
       <c r="D20" s="28"/>
       <c r="E20" s="28"/>
@@ -2646,7 +2654,7 @@
     </row>
     <row r="21" spans="1:38" ht="26.25" customHeight="1">
       <c r="A21" s="14"/>
-      <c r="B21" s="82" t="s">
+      <c r="B21" s="75" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="36"/>
@@ -2688,7 +2696,7 @@
     </row>
     <row r="22" spans="1:38" ht="26.25" customHeight="1">
       <c r="A22" s="14"/>
-      <c r="B22" s="83"/>
+      <c r="B22" s="76"/>
       <c r="C22" s="37"/>
       <c r="D22" s="12"/>
       <c r="E22" s="13"/>
@@ -2728,7 +2736,7 @@
     </row>
     <row r="23" spans="1:38" ht="26.25" customHeight="1" thickBot="1">
       <c r="A23" s="14"/>
-      <c r="B23" s="84"/>
+      <c r="B23" s="77"/>
       <c r="C23" s="38"/>
       <c r="D23" s="18"/>
       <c r="E23" s="19"/>
@@ -2768,17 +2776,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B9:B17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="B5:C7"/>
     <mergeCell ref="I5:AL5"/>
     <mergeCell ref="D5:D7"/>
     <mergeCell ref="E5:E7"/>
     <mergeCell ref="F5:F7"/>
     <mergeCell ref="G5:G7"/>
     <mergeCell ref="H5:H7"/>
+    <mergeCell ref="B9:B17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="B5:C7"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <conditionalFormatting sqref="H21:H23 H9:H16">

</xml_diff>